<commit_message>
ColorControl - Working when width >= height
</commit_message>
<xml_diff>
--- a/doc/ColorPicker.xlsx
+++ b/doc/ColorPicker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ss\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FED647-8F3F-40FD-9E53-0FF2DE59936B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D9FA46-2078-4833-8DDB-FBB145A57664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="3495" windowWidth="28800" windowHeight="15345" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
+    <workbookView xWindow="14535" yWindow="4530" windowWidth="21585" windowHeight="15045" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -467,7 +469,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Color Control - add instead of sub
</commit_message>
<xml_diff>
--- a/doc/ColorPicker.xlsx
+++ b/doc/ColorPicker.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ss\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D9FA46-2078-4833-8DDB-FBB145A57664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DD8E46-234E-4D03-A110-96B210C168C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14535" yWindow="4530" windowWidth="21585" windowHeight="15045" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
+    <workbookView xWindow="18000" yWindow="4605" windowWidth="21585" windowHeight="15045" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gradient" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Height">Sheet1!$B$4</definedName>
-    <definedName name="TargetColor">Sheet1!$B$2</definedName>
-    <definedName name="VerticalStepL">Sheet1!$B$5</definedName>
-    <definedName name="VerticalStepR">Sheet1!$B$6</definedName>
-    <definedName name="Width">Sheet1!$B$3</definedName>
+    <definedName name="BottomLeft">Gradient!$B$4</definedName>
+    <definedName name="BottomRight">Gradient!$B$5</definedName>
+    <definedName name="Height">Gradient!$B$7</definedName>
+    <definedName name="TopLeft">Gradient!$B$2</definedName>
+    <definedName name="TopRight">Gradient!$B$3</definedName>
+    <definedName name="VerticalStepL">Gradient!$B$8</definedName>
+    <definedName name="VerticalStepR">Gradient!$B$9</definedName>
+    <definedName name="Width">Gradient!$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,10 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Target Color</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Width</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>Vertical Step R</t>
+  </si>
+  <si>
+    <t>TopRight</t>
+  </si>
+  <si>
+    <t>TopLeft</t>
+  </si>
+  <si>
+    <t>BottomLeft</t>
+  </si>
+  <si>
+    <t>BottomRight</t>
   </si>
 </sst>
 </file>
@@ -149,7 +161,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -469,7 +481,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -484,16 +496,16 @@
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3">
@@ -548,28 +560,29 @@
     </row>
     <row r="2" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" s="8">
-        <v>150</v>
+        <v>255</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="6">
+        <f>TopLeft</f>
         <v>255</v>
       </c>
       <c r="E2" s="6">
-        <f>TargetColor</f>
-        <v>150</v>
+        <f>TopRight</f>
+        <v>160</v>
       </c>
       <c r="F2" s="6">
         <f>D2-E2</f>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G2" s="6">
-        <f t="shared" ref="G2:G17" si="0">F2/(Width-1)</f>
-        <v>7</v>
+        <f>-F2/(Width-1)</f>
+        <v>-6.333333333333333</v>
       </c>
       <c r="H2" s="3">
         <v>1</v>
@@ -579,64 +592,64 @@
         <v>255</v>
       </c>
       <c r="J2" s="7">
-        <f>I2-$G2</f>
-        <v>248</v>
+        <f>I2+$G2</f>
+        <v>248.66666666666666</v>
       </c>
       <c r="K2" s="7">
-        <f t="shared" ref="K2:X2" si="1">J2-$G2</f>
-        <v>241</v>
+        <f t="shared" ref="K2:X3" si="0">J2+$G2</f>
+        <v>242.33333333333331</v>
       </c>
       <c r="L2" s="7">
-        <f t="shared" si="1"/>
-        <v>234</v>
+        <f t="shared" si="0"/>
+        <v>235.99999999999997</v>
       </c>
       <c r="M2" s="7">
-        <f t="shared" si="1"/>
-        <v>227</v>
+        <f t="shared" si="0"/>
+        <v>229.66666666666663</v>
       </c>
       <c r="N2" s="7">
-        <f t="shared" si="1"/>
-        <v>220</v>
+        <f t="shared" si="0"/>
+        <v>223.33333333333329</v>
       </c>
       <c r="O2" s="7">
-        <f t="shared" si="1"/>
-        <v>213</v>
+        <f t="shared" si="0"/>
+        <v>216.99999999999994</v>
       </c>
       <c r="P2" s="7">
-        <f t="shared" si="1"/>
-        <v>206</v>
+        <f t="shared" si="0"/>
+        <v>210.6666666666666</v>
       </c>
       <c r="Q2" s="7">
-        <f t="shared" si="1"/>
-        <v>199</v>
+        <f t="shared" si="0"/>
+        <v>204.33333333333326</v>
       </c>
       <c r="R2" s="7">
-        <f t="shared" si="1"/>
-        <v>192</v>
+        <f t="shared" si="0"/>
+        <v>197.99999999999991</v>
       </c>
       <c r="S2" s="7">
-        <f t="shared" si="1"/>
-        <v>185</v>
+        <f t="shared" si="0"/>
+        <v>191.66666666666657</v>
       </c>
       <c r="T2" s="7">
-        <f t="shared" si="1"/>
-        <v>178</v>
+        <f t="shared" si="0"/>
+        <v>185.33333333333323</v>
       </c>
       <c r="U2" s="7">
-        <f t="shared" si="1"/>
-        <v>171</v>
+        <f t="shared" si="0"/>
+        <v>178.99999999999989</v>
       </c>
       <c r="V2" s="7">
-        <f t="shared" si="1"/>
-        <v>164</v>
+        <f t="shared" si="0"/>
+        <v>172.66666666666654</v>
       </c>
       <c r="W2" s="7">
-        <f t="shared" si="1"/>
-        <v>157</v>
+        <f t="shared" si="0"/>
+        <v>166.3333333333332</v>
       </c>
       <c r="X2" s="7">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="0"/>
+        <v>159.99999999999986</v>
       </c>
       <c r="Y2" s="3">
         <v>1</v>
@@ -644,96 +657,96 @@
     </row>
     <row r="3" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D17" si="2">D2-VerticalStepL</f>
+        <f t="shared" ref="D3:D17" si="1">D2-VerticalStepL</f>
         <v>238</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E17" si="3">E2-VerticalStepR</f>
-        <v>140</v>
+        <f t="shared" ref="E3:E17" si="2">E2-VerticalStepR</f>
+        <v>149.33333333333334</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" ref="F3:F17" si="4">D3-E3</f>
-        <v>98</v>
+        <f t="shared" ref="F3:F17" si="3">D3-E3</f>
+        <v>88.666666666666657</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" si="0"/>
-        <v>6.5333333333333332</v>
+        <f>-F3/(Width-1)</f>
+        <v>-5.9111111111111105</v>
       </c>
       <c r="H3" s="3">
         <v>2</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3:I17" si="5">D3</f>
+        <f t="shared" ref="I3:I17" si="4">D3</f>
         <v>238</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:X3" si="6">I3-$G3</f>
-        <v>231.46666666666667</v>
+        <f t="shared" ref="J3:X3" si="5">I3+$G3</f>
+        <v>232.0888888888889</v>
       </c>
       <c r="K3" s="7">
-        <f t="shared" si="6"/>
-        <v>224.93333333333334</v>
+        <f t="shared" si="5"/>
+        <v>226.17777777777781</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" si="6"/>
-        <v>218.4</v>
+        <f t="shared" si="5"/>
+        <v>220.26666666666671</v>
       </c>
       <c r="M3" s="7">
-        <f t="shared" si="6"/>
-        <v>211.86666666666667</v>
+        <f t="shared" si="5"/>
+        <v>214.35555555555561</v>
       </c>
       <c r="N3" s="7">
-        <f t="shared" si="6"/>
-        <v>205.33333333333334</v>
+        <f t="shared" si="5"/>
+        <v>208.44444444444451</v>
       </c>
       <c r="O3" s="7">
-        <f t="shared" si="6"/>
-        <v>198.8</v>
+        <f t="shared" si="5"/>
+        <v>202.53333333333342</v>
       </c>
       <c r="P3" s="7">
-        <f t="shared" si="6"/>
-        <v>192.26666666666668</v>
+        <f t="shared" si="5"/>
+        <v>196.62222222222232</v>
       </c>
       <c r="Q3" s="7">
-        <f t="shared" si="6"/>
-        <v>185.73333333333335</v>
+        <f t="shared" si="5"/>
+        <v>190.71111111111122</v>
       </c>
       <c r="R3" s="7">
-        <f t="shared" si="6"/>
-        <v>179.20000000000002</v>
+        <f t="shared" si="5"/>
+        <v>184.80000000000013</v>
       </c>
       <c r="S3" s="7">
-        <f t="shared" si="6"/>
-        <v>172.66666666666669</v>
+        <f t="shared" si="5"/>
+        <v>178.88888888888903</v>
       </c>
       <c r="T3" s="7">
-        <f t="shared" si="6"/>
-        <v>166.13333333333335</v>
+        <f t="shared" si="5"/>
+        <v>172.97777777777793</v>
       </c>
       <c r="U3" s="7">
-        <f t="shared" si="6"/>
-        <v>159.60000000000002</v>
+        <f t="shared" si="5"/>
+        <v>167.06666666666683</v>
       </c>
       <c r="V3" s="7">
-        <f t="shared" si="6"/>
-        <v>153.06666666666669</v>
+        <f t="shared" si="5"/>
+        <v>161.15555555555574</v>
       </c>
       <c r="W3" s="7">
-        <f t="shared" si="6"/>
-        <v>146.53333333333336</v>
+        <f t="shared" si="5"/>
+        <v>155.24444444444464</v>
       </c>
       <c r="X3" s="7">
-        <f t="shared" si="6"/>
-        <v>140.00000000000003</v>
+        <f t="shared" si="5"/>
+        <v>149.33333333333354</v>
       </c>
       <c r="Y3" s="3">
         <v>2</v>
@@ -741,96 +754,96 @@
     </row>
     <row r="4" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B4" s="8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="6">
+        <f t="shared" si="1"/>
+        <v>221</v>
+      </c>
+      <c r="E4" s="6">
         <f t="shared" si="2"/>
-        <v>221</v>
-      </c>
-      <c r="E4" s="6">
+        <v>138.66666666666669</v>
+      </c>
+      <c r="F4" s="6">
         <f t="shared" si="3"/>
-        <v>130</v>
-      </c>
-      <c r="F4" s="6">
-        <f t="shared" si="4"/>
-        <v>91</v>
+        <v>82.333333333333314</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" si="0"/>
-        <v>6.0666666666666664</v>
+        <f>-F4/(Width-1)</f>
+        <v>-5.488888888888888</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>221</v>
       </c>
       <c r="J4" s="7">
-        <f t="shared" ref="J4:X4" si="7">I4-$G4</f>
-        <v>214.93333333333334</v>
+        <f t="shared" ref="J4:X4" si="6">I4+$G4</f>
+        <v>215.51111111111112</v>
       </c>
       <c r="K4" s="7">
-        <f t="shared" si="7"/>
-        <v>208.86666666666667</v>
+        <f t="shared" si="6"/>
+        <v>210.02222222222224</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="7"/>
-        <v>202.8</v>
+        <f t="shared" si="6"/>
+        <v>204.53333333333336</v>
       </c>
       <c r="M4" s="7">
-        <f t="shared" si="7"/>
-        <v>196.73333333333335</v>
+        <f t="shared" si="6"/>
+        <v>199.04444444444448</v>
       </c>
       <c r="N4" s="7">
-        <f t="shared" si="7"/>
-        <v>190.66666666666669</v>
+        <f t="shared" si="6"/>
+        <v>193.5555555555556</v>
       </c>
       <c r="O4" s="7">
-        <f t="shared" si="7"/>
-        <v>184.60000000000002</v>
+        <f t="shared" si="6"/>
+        <v>188.06666666666672</v>
       </c>
       <c r="P4" s="7">
-        <f t="shared" si="7"/>
-        <v>178.53333333333336</v>
+        <f t="shared" si="6"/>
+        <v>182.57777777777784</v>
       </c>
       <c r="Q4" s="7">
-        <f t="shared" si="7"/>
-        <v>172.4666666666667</v>
+        <f t="shared" si="6"/>
+        <v>177.08888888888896</v>
       </c>
       <c r="R4" s="7">
-        <f t="shared" si="7"/>
-        <v>166.40000000000003</v>
+        <f t="shared" si="6"/>
+        <v>171.60000000000008</v>
       </c>
       <c r="S4" s="7">
-        <f t="shared" si="7"/>
-        <v>160.33333333333337</v>
+        <f t="shared" si="6"/>
+        <v>166.1111111111112</v>
       </c>
       <c r="T4" s="7">
-        <f t="shared" si="7"/>
-        <v>154.26666666666671</v>
+        <f t="shared" si="6"/>
+        <v>160.62222222222232</v>
       </c>
       <c r="U4" s="7">
-        <f t="shared" si="7"/>
-        <v>148.20000000000005</v>
+        <f t="shared" si="6"/>
+        <v>155.13333333333344</v>
       </c>
       <c r="V4" s="7">
-        <f t="shared" si="7"/>
-        <v>142.13333333333338</v>
+        <f t="shared" si="6"/>
+        <v>149.64444444444456</v>
       </c>
       <c r="W4" s="7">
-        <f t="shared" si="7"/>
-        <v>136.06666666666672</v>
+        <f t="shared" si="6"/>
+        <v>144.15555555555568</v>
       </c>
       <c r="X4" s="7">
-        <f t="shared" si="7"/>
-        <v>130.00000000000006</v>
+        <f t="shared" si="6"/>
+        <v>138.6666666666668</v>
       </c>
       <c r="Y4" s="3">
         <v>3</v>
@@ -838,97 +851,96 @@
     </row>
     <row r="5" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6">
-        <f>D2/(Height-1)</f>
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="6">
+        <f t="shared" si="1"/>
+        <v>204</v>
+      </c>
+      <c r="E5" s="6">
         <f t="shared" si="2"/>
-        <v>204</v>
-      </c>
-      <c r="E5" s="6">
+        <v>128.00000000000003</v>
+      </c>
+      <c r="F5" s="6">
         <f t="shared" si="3"/>
-        <v>120</v>
-      </c>
-      <c r="F5" s="6">
-        <f t="shared" si="4"/>
-        <v>84</v>
+        <v>75.999999999999972</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="0"/>
-        <v>5.6</v>
+        <f>-F5/(Width-1)</f>
+        <v>-5.0666666666666647</v>
       </c>
       <c r="H5" s="3">
         <v>4</v>
       </c>
       <c r="I5" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>204</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" ref="J5:X5" si="8">I5-$G5</f>
-        <v>198.4</v>
+        <f t="shared" ref="J5:X5" si="7">I5+$G5</f>
+        <v>198.93333333333334</v>
       </c>
       <c r="K5" s="7">
-        <f t="shared" si="8"/>
-        <v>192.8</v>
+        <f t="shared" si="7"/>
+        <v>193.86666666666667</v>
       </c>
       <c r="L5" s="7">
-        <f t="shared" si="8"/>
-        <v>187.20000000000002</v>
+        <f t="shared" si="7"/>
+        <v>188.8</v>
       </c>
       <c r="M5" s="7">
-        <f t="shared" si="8"/>
-        <v>181.60000000000002</v>
+        <f t="shared" si="7"/>
+        <v>183.73333333333335</v>
       </c>
       <c r="N5" s="7">
-        <f t="shared" si="8"/>
-        <v>176.00000000000003</v>
+        <f t="shared" si="7"/>
+        <v>178.66666666666669</v>
       </c>
       <c r="O5" s="7">
-        <f t="shared" si="8"/>
-        <v>170.40000000000003</v>
+        <f t="shared" si="7"/>
+        <v>173.60000000000002</v>
       </c>
       <c r="P5" s="7">
-        <f t="shared" si="8"/>
-        <v>164.80000000000004</v>
+        <f t="shared" si="7"/>
+        <v>168.53333333333336</v>
       </c>
       <c r="Q5" s="7">
-        <f t="shared" si="8"/>
-        <v>159.20000000000005</v>
+        <f t="shared" si="7"/>
+        <v>163.4666666666667</v>
       </c>
       <c r="R5" s="7">
-        <f t="shared" si="8"/>
-        <v>153.60000000000005</v>
+        <f t="shared" si="7"/>
+        <v>158.40000000000003</v>
       </c>
       <c r="S5" s="7">
-        <f t="shared" si="8"/>
-        <v>148.00000000000006</v>
+        <f t="shared" si="7"/>
+        <v>153.33333333333337</v>
       </c>
       <c r="T5" s="7">
-        <f t="shared" si="8"/>
-        <v>142.40000000000006</v>
+        <f t="shared" si="7"/>
+        <v>148.26666666666671</v>
       </c>
       <c r="U5" s="7">
-        <f t="shared" si="8"/>
-        <v>136.80000000000007</v>
+        <f t="shared" si="7"/>
+        <v>143.20000000000005</v>
       </c>
       <c r="V5" s="7">
-        <f t="shared" si="8"/>
-        <v>131.20000000000007</v>
+        <f t="shared" si="7"/>
+        <v>138.13333333333338</v>
       </c>
       <c r="W5" s="7">
-        <f t="shared" si="8"/>
-        <v>125.60000000000008</v>
+        <f t="shared" si="7"/>
+        <v>133.06666666666672</v>
       </c>
       <c r="X5" s="7">
-        <f t="shared" si="8"/>
-        <v>120.00000000000009</v>
+        <f t="shared" si="7"/>
+        <v>128.00000000000006</v>
       </c>
       <c r="Y5" s="3">
         <v>4</v>
@@ -936,370 +948,389 @@
     </row>
     <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
-        <f>E2/(Height - 1)</f>
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>16</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="6">
+        <f t="shared" si="1"/>
+        <v>187</v>
+      </c>
+      <c r="E6" s="6">
         <f t="shared" si="2"/>
-        <v>187</v>
-      </c>
-      <c r="E6" s="6">
+        <v>117.33333333333336</v>
+      </c>
+      <c r="F6" s="6">
         <f t="shared" si="3"/>
-        <v>110</v>
-      </c>
-      <c r="F6" s="6">
-        <f t="shared" si="4"/>
-        <v>77</v>
+        <v>69.666666666666643</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="0"/>
-        <v>5.1333333333333337</v>
+        <f>-F6/(Width-1)</f>
+        <v>-4.644444444444443</v>
       </c>
       <c r="H6" s="3">
         <v>5</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>187</v>
       </c>
       <c r="J6" s="7">
-        <f t="shared" ref="J6:X6" si="9">I6-$G6</f>
-        <v>181.86666666666667</v>
+        <f t="shared" ref="J6:X6" si="8">I6+$G6</f>
+        <v>182.35555555555555</v>
       </c>
       <c r="K6" s="7">
-        <f t="shared" si="9"/>
-        <v>176.73333333333335</v>
+        <f t="shared" si="8"/>
+        <v>177.71111111111111</v>
       </c>
       <c r="L6" s="7">
-        <f t="shared" si="9"/>
-        <v>171.60000000000002</v>
+        <f t="shared" si="8"/>
+        <v>173.06666666666666</v>
       </c>
       <c r="M6" s="7">
-        <f t="shared" si="9"/>
-        <v>166.4666666666667</v>
+        <f t="shared" si="8"/>
+        <v>168.42222222222222</v>
       </c>
       <c r="N6" s="7">
-        <f t="shared" si="9"/>
-        <v>161.33333333333337</v>
+        <f t="shared" si="8"/>
+        <v>163.77777777777777</v>
       </c>
       <c r="O6" s="7">
-        <f t="shared" si="9"/>
-        <v>156.20000000000005</v>
+        <f t="shared" si="8"/>
+        <v>159.13333333333333</v>
       </c>
       <c r="P6" s="7">
-        <f t="shared" si="9"/>
-        <v>151.06666666666672</v>
+        <f t="shared" si="8"/>
+        <v>154.48888888888888</v>
       </c>
       <c r="Q6" s="7">
-        <f t="shared" si="9"/>
-        <v>145.93333333333339</v>
+        <f t="shared" si="8"/>
+        <v>149.84444444444443</v>
       </c>
       <c r="R6" s="7">
-        <f t="shared" si="9"/>
-        <v>140.80000000000007</v>
+        <f t="shared" si="8"/>
+        <v>145.19999999999999</v>
       </c>
       <c r="S6" s="7">
-        <f t="shared" si="9"/>
-        <v>135.66666666666674</v>
+        <f t="shared" si="8"/>
+        <v>140.55555555555554</v>
       </c>
       <c r="T6" s="7">
-        <f t="shared" si="9"/>
-        <v>130.53333333333342</v>
+        <f t="shared" si="8"/>
+        <v>135.9111111111111</v>
       </c>
       <c r="U6" s="7">
-        <f t="shared" si="9"/>
-        <v>125.40000000000008</v>
+        <f t="shared" si="8"/>
+        <v>131.26666666666665</v>
       </c>
       <c r="V6" s="7">
-        <f t="shared" si="9"/>
-        <v>120.26666666666674</v>
+        <f t="shared" si="8"/>
+        <v>126.62222222222221</v>
       </c>
       <c r="W6" s="7">
-        <f t="shared" si="9"/>
-        <v>115.1333333333334</v>
+        <f t="shared" si="8"/>
+        <v>121.97777777777776</v>
       </c>
       <c r="X6" s="7">
-        <f t="shared" si="9"/>
-        <v>110.00000000000006</v>
+        <f t="shared" si="8"/>
+        <v>117.33333333333331</v>
       </c>
       <c r="Y6" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>16</v>
+      </c>
       <c r="C7" s="3">
         <v>6</v>
       </c>
       <c r="D7" s="6">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+      <c r="E7" s="6">
         <f t="shared" si="2"/>
-        <v>170</v>
-      </c>
-      <c r="E7" s="6">
+        <v>106.66666666666669</v>
+      </c>
+      <c r="F7" s="6">
         <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <v>63.333333333333314</v>
       </c>
       <c r="G7" s="6">
-        <f t="shared" si="0"/>
-        <v>4.666666666666667</v>
+        <f>-F7/(Width-1)</f>
+        <v>-4.2222222222222205</v>
       </c>
       <c r="H7" s="3">
         <v>6</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>170</v>
       </c>
       <c r="J7" s="7">
-        <f t="shared" ref="J7:X7" si="10">I7-$G7</f>
-        <v>165.33333333333334</v>
+        <f t="shared" ref="J7:X7" si="9">I7+$G7</f>
+        <v>165.77777777777777</v>
       </c>
       <c r="K7" s="7">
-        <f t="shared" si="10"/>
-        <v>160.66666666666669</v>
+        <f t="shared" si="9"/>
+        <v>161.55555555555554</v>
       </c>
       <c r="L7" s="7">
-        <f t="shared" si="10"/>
-        <v>156.00000000000003</v>
+        <f t="shared" si="9"/>
+        <v>157.33333333333331</v>
       </c>
       <c r="M7" s="7">
-        <f t="shared" si="10"/>
-        <v>151.33333333333337</v>
+        <f t="shared" si="9"/>
+        <v>153.11111111111109</v>
       </c>
       <c r="N7" s="7">
-        <f t="shared" si="10"/>
-        <v>146.66666666666671</v>
+        <f t="shared" si="9"/>
+        <v>148.88888888888886</v>
       </c>
       <c r="O7" s="7">
-        <f t="shared" si="10"/>
-        <v>142.00000000000006</v>
+        <f t="shared" si="9"/>
+        <v>144.66666666666663</v>
       </c>
       <c r="P7" s="7">
-        <f t="shared" si="10"/>
-        <v>137.3333333333334</v>
+        <f t="shared" si="9"/>
+        <v>140.4444444444444</v>
       </c>
       <c r="Q7" s="7">
-        <f t="shared" si="10"/>
-        <v>132.66666666666674</v>
+        <f t="shared" si="9"/>
+        <v>136.22222222222217</v>
       </c>
       <c r="R7" s="7">
-        <f t="shared" si="10"/>
-        <v>128.00000000000009</v>
+        <f t="shared" si="9"/>
+        <v>131.99999999999994</v>
       </c>
       <c r="S7" s="7">
-        <f t="shared" si="10"/>
-        <v>123.33333333333341</v>
+        <f t="shared" si="9"/>
+        <v>127.77777777777773</v>
       </c>
       <c r="T7" s="7">
-        <f t="shared" si="10"/>
-        <v>118.66666666666674</v>
+        <f t="shared" si="9"/>
+        <v>123.55555555555551</v>
       </c>
       <c r="U7" s="7">
-        <f t="shared" si="10"/>
-        <v>114.00000000000007</v>
+        <f t="shared" si="9"/>
+        <v>119.3333333333333</v>
       </c>
       <c r="V7" s="7">
-        <f t="shared" si="10"/>
-        <v>109.3333333333334</v>
+        <f t="shared" si="9"/>
+        <v>115.11111111111109</v>
       </c>
       <c r="W7" s="7">
-        <f t="shared" si="10"/>
-        <v>104.66666666666673</v>
+        <f t="shared" si="9"/>
+        <v>110.88888888888887</v>
       </c>
       <c r="X7" s="7">
-        <f t="shared" si="10"/>
-        <v>100.00000000000006</v>
+        <f t="shared" si="9"/>
+        <v>106.66666666666666</v>
       </c>
       <c r="Y7" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <f>(TopLeft-BottomLeft)/(Height-1)</f>
+        <v>17</v>
+      </c>
       <c r="C8" s="3">
         <v>7</v>
       </c>
       <c r="D8" s="6">
+        <f t="shared" si="1"/>
+        <v>153</v>
+      </c>
+      <c r="E8" s="6">
         <f t="shared" si="2"/>
-        <v>153</v>
-      </c>
-      <c r="E8" s="6">
+        <v>96.000000000000014</v>
+      </c>
+      <c r="F8" s="6">
         <f t="shared" si="3"/>
-        <v>90</v>
-      </c>
-      <c r="F8" s="6">
-        <f t="shared" si="4"/>
-        <v>63</v>
+        <v>56.999999999999986</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="0"/>
-        <v>4.2</v>
+        <f>-F8/(Width-1)</f>
+        <v>-3.7999999999999989</v>
       </c>
       <c r="H8" s="3">
         <v>7</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>153</v>
       </c>
       <c r="J8" s="7">
-        <f t="shared" ref="J8:X8" si="11">I8-$G8</f>
-        <v>148.80000000000001</v>
+        <f t="shared" ref="J8:X8" si="10">I8+$G8</f>
+        <v>149.19999999999999</v>
       </c>
       <c r="K8" s="7">
-        <f t="shared" si="11"/>
-        <v>144.60000000000002</v>
+        <f t="shared" si="10"/>
+        <v>145.39999999999998</v>
       </c>
       <c r="L8" s="7">
-        <f t="shared" si="11"/>
-        <v>140.40000000000003</v>
+        <f t="shared" si="10"/>
+        <v>141.59999999999997</v>
       </c>
       <c r="M8" s="7">
-        <f t="shared" si="11"/>
-        <v>136.20000000000005</v>
+        <f t="shared" si="10"/>
+        <v>137.79999999999995</v>
       </c>
       <c r="N8" s="7">
-        <f t="shared" si="11"/>
-        <v>132.00000000000006</v>
+        <f t="shared" si="10"/>
+        <v>133.99999999999994</v>
       </c>
       <c r="O8" s="7">
-        <f t="shared" si="11"/>
-        <v>127.80000000000005</v>
+        <f t="shared" si="10"/>
+        <v>130.19999999999993</v>
       </c>
       <c r="P8" s="7">
-        <f t="shared" si="11"/>
-        <v>123.60000000000005</v>
+        <f t="shared" si="10"/>
+        <v>126.39999999999993</v>
       </c>
       <c r="Q8" s="7">
-        <f t="shared" si="11"/>
-        <v>119.40000000000005</v>
+        <f t="shared" si="10"/>
+        <v>122.59999999999994</v>
       </c>
       <c r="R8" s="7">
-        <f t="shared" si="11"/>
-        <v>115.20000000000005</v>
+        <f t="shared" si="10"/>
+        <v>118.79999999999994</v>
       </c>
       <c r="S8" s="7">
-        <f t="shared" si="11"/>
-        <v>111.00000000000004</v>
+        <f t="shared" si="10"/>
+        <v>114.99999999999994</v>
       </c>
       <c r="T8" s="7">
-        <f t="shared" si="11"/>
-        <v>106.80000000000004</v>
+        <f t="shared" si="10"/>
+        <v>111.19999999999995</v>
       </c>
       <c r="U8" s="7">
-        <f t="shared" si="11"/>
-        <v>102.60000000000004</v>
+        <f t="shared" si="10"/>
+        <v>107.39999999999995</v>
       </c>
       <c r="V8" s="7">
-        <f t="shared" si="11"/>
-        <v>98.400000000000034</v>
+        <f t="shared" si="10"/>
+        <v>103.59999999999995</v>
       </c>
       <c r="W8" s="7">
-        <f t="shared" si="11"/>
-        <v>94.200000000000031</v>
+        <f t="shared" si="10"/>
+        <v>99.799999999999955</v>
       </c>
       <c r="X8" s="7">
-        <f t="shared" si="11"/>
-        <v>90.000000000000028</v>
+        <f t="shared" si="10"/>
+        <v>95.999999999999957</v>
       </c>
       <c r="Y8" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <f>(TopRight-BottomRight)/(Height - 1)</f>
+        <v>10.666666666666666</v>
+      </c>
       <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="6">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+      <c r="E9" s="6">
         <f t="shared" si="2"/>
-        <v>136</v>
-      </c>
-      <c r="E9" s="6">
+        <v>85.333333333333343</v>
+      </c>
+      <c r="F9" s="6">
         <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-      <c r="F9" s="6">
-        <f t="shared" si="4"/>
-        <v>56</v>
+        <v>50.666666666666657</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7333333333333334</v>
+        <f>-F9/(Width-1)</f>
+        <v>-3.3777777777777773</v>
       </c>
       <c r="H9" s="3">
         <v>8</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>136</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" ref="J9:X9" si="12">I9-$G9</f>
-        <v>132.26666666666668</v>
+        <f t="shared" ref="J9:X9" si="11">I9+$G9</f>
+        <v>132.62222222222223</v>
       </c>
       <c r="K9" s="7">
-        <f t="shared" si="12"/>
-        <v>128.53333333333336</v>
+        <f t="shared" si="11"/>
+        <v>129.24444444444447</v>
       </c>
       <c r="L9" s="7">
-        <f t="shared" si="12"/>
-        <v>124.80000000000003</v>
+        <f t="shared" si="11"/>
+        <v>125.86666666666669</v>
       </c>
       <c r="M9" s="7">
-        <f t="shared" si="12"/>
-        <v>121.06666666666669</v>
+        <f t="shared" si="11"/>
+        <v>122.48888888888891</v>
       </c>
       <c r="N9" s="7">
-        <f t="shared" si="12"/>
-        <v>117.33333333333336</v>
+        <f t="shared" si="11"/>
+        <v>119.11111111111113</v>
       </c>
       <c r="O9" s="7">
-        <f t="shared" si="12"/>
-        <v>113.60000000000002</v>
+        <f t="shared" si="11"/>
+        <v>115.73333333333335</v>
       </c>
       <c r="P9" s="7">
-        <f t="shared" si="12"/>
-        <v>109.86666666666669</v>
+        <f t="shared" si="11"/>
+        <v>112.35555555555557</v>
       </c>
       <c r="Q9" s="7">
-        <f t="shared" si="12"/>
-        <v>106.13333333333335</v>
+        <f t="shared" si="11"/>
+        <v>108.97777777777779</v>
       </c>
       <c r="R9" s="7">
-        <f t="shared" si="12"/>
-        <v>102.40000000000002</v>
+        <f t="shared" si="11"/>
+        <v>105.60000000000001</v>
       </c>
       <c r="S9" s="7">
-        <f t="shared" si="12"/>
-        <v>98.666666666666686</v>
+        <f t="shared" si="11"/>
+        <v>102.22222222222223</v>
       </c>
       <c r="T9" s="7">
-        <f t="shared" si="12"/>
-        <v>94.933333333333351</v>
+        <f t="shared" si="11"/>
+        <v>98.844444444444449</v>
       </c>
       <c r="U9" s="7">
-        <f t="shared" si="12"/>
-        <v>91.200000000000017</v>
+        <f t="shared" si="11"/>
+        <v>95.466666666666669</v>
       </c>
       <c r="V9" s="7">
-        <f t="shared" si="12"/>
-        <v>87.466666666666683</v>
+        <f t="shared" si="11"/>
+        <v>92.088888888888889</v>
       </c>
       <c r="W9" s="7">
-        <f t="shared" si="12"/>
-        <v>83.733333333333348</v>
+        <f t="shared" si="11"/>
+        <v>88.711111111111109</v>
       </c>
       <c r="X9" s="7">
-        <f t="shared" si="12"/>
-        <v>80.000000000000014</v>
+        <f t="shared" si="11"/>
+        <v>85.333333333333329</v>
       </c>
       <c r="Y9" s="3">
         <v>8</v>
@@ -1310,87 +1341,87 @@
         <v>9</v>
       </c>
       <c r="D10" s="6">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="E10" s="6">
         <f t="shared" si="2"/>
-        <v>119</v>
-      </c>
-      <c r="E10" s="6">
+        <v>74.666666666666671</v>
+      </c>
+      <c r="F10" s="6">
         <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="F10" s="6">
-        <f t="shared" si="4"/>
-        <v>49</v>
+        <v>44.333333333333329</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="0"/>
-        <v>3.2666666666666666</v>
+        <f>-F10/(Width-1)</f>
+        <v>-2.9555555555555553</v>
       </c>
       <c r="H10" s="3">
         <v>9</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>119</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" ref="J10:X10" si="13">I10-$G10</f>
-        <v>115.73333333333333</v>
+        <f t="shared" ref="J10:X10" si="12">I10+$G10</f>
+        <v>116.04444444444445</v>
       </c>
       <c r="K10" s="7">
-        <f t="shared" si="13"/>
-        <v>112.46666666666667</v>
+        <f t="shared" si="12"/>
+        <v>113.0888888888889</v>
       </c>
       <c r="L10" s="7">
-        <f t="shared" si="13"/>
-        <v>109.2</v>
+        <f t="shared" si="12"/>
+        <v>110.13333333333335</v>
       </c>
       <c r="M10" s="7">
-        <f t="shared" si="13"/>
-        <v>105.93333333333334</v>
+        <f t="shared" si="12"/>
+        <v>107.17777777777781</v>
       </c>
       <c r="N10" s="7">
-        <f t="shared" si="13"/>
-        <v>102.66666666666667</v>
+        <f t="shared" si="12"/>
+        <v>104.22222222222226</v>
       </c>
       <c r="O10" s="7">
-        <f t="shared" si="13"/>
-        <v>99.4</v>
+        <f t="shared" si="12"/>
+        <v>101.26666666666671</v>
       </c>
       <c r="P10" s="7">
-        <f t="shared" si="13"/>
-        <v>96.13333333333334</v>
+        <f t="shared" si="12"/>
+        <v>98.31111111111116</v>
       </c>
       <c r="Q10" s="7">
-        <f t="shared" si="13"/>
-        <v>92.866666666666674</v>
+        <f t="shared" si="12"/>
+        <v>95.355555555555611</v>
       </c>
       <c r="R10" s="7">
-        <f t="shared" si="13"/>
-        <v>89.600000000000009</v>
+        <f t="shared" si="12"/>
+        <v>92.400000000000063</v>
       </c>
       <c r="S10" s="7">
-        <f t="shared" si="13"/>
-        <v>86.333333333333343</v>
+        <f t="shared" si="12"/>
+        <v>89.444444444444514</v>
       </c>
       <c r="T10" s="7">
-        <f t="shared" si="13"/>
-        <v>83.066666666666677</v>
+        <f t="shared" si="12"/>
+        <v>86.488888888888965</v>
       </c>
       <c r="U10" s="7">
-        <f t="shared" si="13"/>
-        <v>79.800000000000011</v>
+        <f t="shared" si="12"/>
+        <v>83.533333333333417</v>
       </c>
       <c r="V10" s="7">
-        <f t="shared" si="13"/>
-        <v>76.533333333333346</v>
+        <f t="shared" si="12"/>
+        <v>80.577777777777868</v>
       </c>
       <c r="W10" s="7">
-        <f t="shared" si="13"/>
-        <v>73.26666666666668</v>
+        <f t="shared" si="12"/>
+        <v>77.622222222222319</v>
       </c>
       <c r="X10" s="7">
-        <f t="shared" si="13"/>
-        <v>70.000000000000014</v>
+        <f t="shared" si="12"/>
+        <v>74.666666666666771</v>
       </c>
       <c r="Y10" s="3">
         <v>9</v>
@@ -1401,87 +1432,87 @@
         <v>10</v>
       </c>
       <c r="D11" s="6">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="E11" s="6">
         <f t="shared" si="2"/>
-        <v>102</v>
-      </c>
-      <c r="E11" s="6">
+        <v>64</v>
+      </c>
+      <c r="F11" s="6">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="F11" s="6">
-        <f t="shared" si="4"/>
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
+        <f>-F11/(Width-1)</f>
+        <v>-2.5333333333333332</v>
       </c>
       <c r="H11" s="3">
         <v>10</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" ref="J11:X11" si="14">I11-$G11</f>
-        <v>99.2</v>
+        <f t="shared" ref="J11:X11" si="13">I11+$G11</f>
+        <v>99.466666666666669</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="14"/>
-        <v>96.4</v>
+        <f t="shared" si="13"/>
+        <v>96.933333333333337</v>
       </c>
       <c r="L11" s="7">
-        <f t="shared" si="14"/>
-        <v>93.600000000000009</v>
+        <f t="shared" si="13"/>
+        <v>94.4</v>
       </c>
       <c r="M11" s="7">
-        <f t="shared" si="14"/>
-        <v>90.800000000000011</v>
+        <f t="shared" si="13"/>
+        <v>91.866666666666674</v>
       </c>
       <c r="N11" s="7">
-        <f t="shared" si="14"/>
-        <v>88.000000000000014</v>
+        <f t="shared" si="13"/>
+        <v>89.333333333333343</v>
       </c>
       <c r="O11" s="7">
-        <f t="shared" si="14"/>
-        <v>85.200000000000017</v>
+        <f t="shared" si="13"/>
+        <v>86.800000000000011</v>
       </c>
       <c r="P11" s="7">
-        <f t="shared" si="14"/>
-        <v>82.40000000000002</v>
+        <f t="shared" si="13"/>
+        <v>84.26666666666668</v>
       </c>
       <c r="Q11" s="7">
-        <f t="shared" si="14"/>
-        <v>79.600000000000023</v>
+        <f t="shared" si="13"/>
+        <v>81.733333333333348</v>
       </c>
       <c r="R11" s="7">
-        <f t="shared" si="14"/>
-        <v>76.800000000000026</v>
+        <f t="shared" si="13"/>
+        <v>79.200000000000017</v>
       </c>
       <c r="S11" s="7">
-        <f t="shared" si="14"/>
-        <v>74.000000000000028</v>
+        <f t="shared" si="13"/>
+        <v>76.666666666666686</v>
       </c>
       <c r="T11" s="7">
-        <f t="shared" si="14"/>
-        <v>71.200000000000031</v>
+        <f t="shared" si="13"/>
+        <v>74.133333333333354</v>
       </c>
       <c r="U11" s="7">
-        <f t="shared" si="14"/>
-        <v>68.400000000000034</v>
+        <f t="shared" si="13"/>
+        <v>71.600000000000023</v>
       </c>
       <c r="V11" s="7">
-        <f t="shared" si="14"/>
-        <v>65.600000000000037</v>
+        <f t="shared" si="13"/>
+        <v>69.066666666666691</v>
       </c>
       <c r="W11" s="7">
-        <f t="shared" si="14"/>
-        <v>62.80000000000004</v>
+        <f t="shared" si="13"/>
+        <v>66.53333333333336</v>
       </c>
       <c r="X11" s="7">
-        <f t="shared" si="14"/>
-        <v>60.000000000000043</v>
+        <f t="shared" si="13"/>
+        <v>64.000000000000028</v>
       </c>
       <c r="Y11" s="3">
         <v>10</v>
@@ -1492,87 +1523,87 @@
         <v>11</v>
       </c>
       <c r="D12" s="6">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="E12" s="6">
         <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="E12" s="6">
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F12" s="6">
         <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="F12" s="6">
-        <f t="shared" si="4"/>
-        <v>35</v>
+        <v>31.666666666666664</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="0"/>
-        <v>2.3333333333333335</v>
+        <f>-F12/(Width-1)</f>
+        <v>-2.1111111111111112</v>
       </c>
       <c r="H12" s="3">
         <v>11</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" ref="J12:X12" si="15">I12-$G12</f>
-        <v>82.666666666666671</v>
+        <f t="shared" ref="J12:X12" si="14">I12+$G12</f>
+        <v>82.888888888888886</v>
       </c>
       <c r="K12" s="7">
-        <f t="shared" si="15"/>
-        <v>80.333333333333343</v>
+        <f t="shared" si="14"/>
+        <v>80.777777777777771</v>
       </c>
       <c r="L12" s="7">
-        <f t="shared" si="15"/>
-        <v>78.000000000000014</v>
+        <f t="shared" si="14"/>
+        <v>78.666666666666657</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" si="15"/>
-        <v>75.666666666666686</v>
+        <f t="shared" si="14"/>
+        <v>76.555555555555543</v>
       </c>
       <c r="N12" s="7">
-        <f t="shared" si="15"/>
-        <v>73.333333333333357</v>
+        <f t="shared" si="14"/>
+        <v>74.444444444444429</v>
       </c>
       <c r="O12" s="7">
-        <f t="shared" si="15"/>
-        <v>71.000000000000028</v>
+        <f t="shared" si="14"/>
+        <v>72.333333333333314</v>
       </c>
       <c r="P12" s="7">
-        <f t="shared" si="15"/>
-        <v>68.6666666666667</v>
+        <f t="shared" si="14"/>
+        <v>70.2222222222222</v>
       </c>
       <c r="Q12" s="7">
-        <f t="shared" si="15"/>
-        <v>66.333333333333371</v>
+        <f t="shared" si="14"/>
+        <v>68.111111111111086</v>
       </c>
       <c r="R12" s="7">
-        <f t="shared" si="15"/>
-        <v>64.000000000000043</v>
+        <f t="shared" si="14"/>
+        <v>65.999999999999972</v>
       </c>
       <c r="S12" s="7">
-        <f t="shared" si="15"/>
-        <v>61.666666666666707</v>
+        <f t="shared" si="14"/>
+        <v>63.888888888888857</v>
       </c>
       <c r="T12" s="7">
-        <f t="shared" si="15"/>
-        <v>59.333333333333371</v>
+        <f t="shared" si="14"/>
+        <v>61.777777777777743</v>
       </c>
       <c r="U12" s="7">
-        <f t="shared" si="15"/>
-        <v>57.000000000000036</v>
+        <f t="shared" si="14"/>
+        <v>59.666666666666629</v>
       </c>
       <c r="V12" s="7">
-        <f t="shared" si="15"/>
-        <v>54.6666666666667</v>
+        <f t="shared" si="14"/>
+        <v>57.555555555555515</v>
       </c>
       <c r="W12" s="7">
-        <f t="shared" si="15"/>
-        <v>52.333333333333364</v>
+        <f t="shared" si="14"/>
+        <v>55.4444444444444</v>
       </c>
       <c r="X12" s="7">
-        <f t="shared" si="15"/>
-        <v>50.000000000000028</v>
+        <f t="shared" si="14"/>
+        <v>53.333333333333286</v>
       </c>
       <c r="Y12" s="3">
         <v>11</v>
@@ -1583,87 +1614,87 @@
         <v>12</v>
       </c>
       <c r="D13" s="6">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="E13" s="6">
         <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="E13" s="6">
+        <v>42.666666666666671</v>
+      </c>
+      <c r="F13" s="6">
         <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="F13" s="6">
-        <f t="shared" si="4"/>
-        <v>28</v>
+        <v>25.333333333333329</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="0"/>
-        <v>1.8666666666666667</v>
+        <f>-F13/(Width-1)</f>
+        <v>-1.6888888888888887</v>
       </c>
       <c r="H13" s="3">
         <v>12</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" ref="J13:X13" si="16">I13-$G13</f>
-        <v>66.13333333333334</v>
+        <f t="shared" ref="J13:X13" si="15">I13+$G13</f>
+        <v>66.311111111111117</v>
       </c>
       <c r="K13" s="7">
-        <f t="shared" si="16"/>
-        <v>64.26666666666668</v>
+        <f t="shared" si="15"/>
+        <v>64.622222222222234</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" si="16"/>
-        <v>62.400000000000013</v>
+        <f t="shared" si="15"/>
+        <v>62.933333333333344</v>
       </c>
       <c r="M13" s="7">
-        <f t="shared" si="16"/>
-        <v>60.533333333333346</v>
+        <f t="shared" si="15"/>
+        <v>61.244444444444454</v>
       </c>
       <c r="N13" s="7">
-        <f t="shared" si="16"/>
-        <v>58.666666666666679</v>
+        <f t="shared" si="15"/>
+        <v>59.555555555555564</v>
       </c>
       <c r="O13" s="7">
-        <f t="shared" si="16"/>
-        <v>56.800000000000011</v>
+        <f t="shared" si="15"/>
+        <v>57.866666666666674</v>
       </c>
       <c r="P13" s="7">
-        <f t="shared" si="16"/>
-        <v>54.933333333333344</v>
+        <f t="shared" si="15"/>
+        <v>56.177777777777784</v>
       </c>
       <c r="Q13" s="7">
-        <f t="shared" si="16"/>
-        <v>53.066666666666677</v>
+        <f t="shared" si="15"/>
+        <v>54.488888888888894</v>
       </c>
       <c r="R13" s="7">
-        <f t="shared" si="16"/>
-        <v>51.20000000000001</v>
+        <f t="shared" si="15"/>
+        <v>52.800000000000004</v>
       </c>
       <c r="S13" s="7">
-        <f t="shared" si="16"/>
-        <v>49.333333333333343</v>
+        <f t="shared" si="15"/>
+        <v>51.111111111111114</v>
       </c>
       <c r="T13" s="7">
-        <f t="shared" si="16"/>
-        <v>47.466666666666676</v>
+        <f t="shared" si="15"/>
+        <v>49.422222222222224</v>
       </c>
       <c r="U13" s="7">
-        <f t="shared" si="16"/>
-        <v>45.600000000000009</v>
+        <f t="shared" si="15"/>
+        <v>47.733333333333334</v>
       </c>
       <c r="V13" s="7">
-        <f t="shared" si="16"/>
-        <v>43.733333333333341</v>
+        <f t="shared" si="15"/>
+        <v>46.044444444444444</v>
       </c>
       <c r="W13" s="7">
-        <f t="shared" si="16"/>
-        <v>41.866666666666674</v>
+        <f t="shared" si="15"/>
+        <v>44.355555555555554</v>
       </c>
       <c r="X13" s="7">
-        <f t="shared" si="16"/>
-        <v>40.000000000000007</v>
+        <f t="shared" si="15"/>
+        <v>42.666666666666664</v>
       </c>
       <c r="Y13" s="3">
         <v>12</v>
@@ -1674,87 +1705,87 @@
         <v>13</v>
       </c>
       <c r="D14" s="6">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E14" s="6">
         <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-      <c r="E14" s="6">
+        <v>32.000000000000007</v>
+      </c>
+      <c r="F14" s="6">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="F14" s="6">
-        <f t="shared" si="4"/>
-        <v>21</v>
+        <v>18.999999999999993</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
+        <f>-F14/(Width-1)</f>
+        <v>-1.2666666666666662</v>
       </c>
       <c r="H14" s="3">
         <v>13</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" ref="J14:X14" si="17">I14-$G14</f>
-        <v>49.6</v>
+        <f t="shared" ref="J14:X14" si="16">I14+$G14</f>
+        <v>49.733333333333334</v>
       </c>
       <c r="K14" s="7">
-        <f t="shared" si="17"/>
-        <v>48.2</v>
+        <f t="shared" si="16"/>
+        <v>48.466666666666669</v>
       </c>
       <c r="L14" s="7">
-        <f t="shared" si="17"/>
-        <v>46.800000000000004</v>
+        <f t="shared" si="16"/>
+        <v>47.2</v>
       </c>
       <c r="M14" s="7">
-        <f t="shared" si="17"/>
-        <v>45.400000000000006</v>
+        <f t="shared" si="16"/>
+        <v>45.933333333333337</v>
       </c>
       <c r="N14" s="7">
-        <f t="shared" si="17"/>
-        <v>44.000000000000007</v>
+        <f t="shared" si="16"/>
+        <v>44.666666666666671</v>
       </c>
       <c r="O14" s="7">
-        <f t="shared" si="17"/>
-        <v>42.600000000000009</v>
+        <f t="shared" si="16"/>
+        <v>43.400000000000006</v>
       </c>
       <c r="P14" s="7">
-        <f t="shared" si="17"/>
-        <v>41.20000000000001</v>
+        <f t="shared" si="16"/>
+        <v>42.13333333333334</v>
       </c>
       <c r="Q14" s="7">
-        <f t="shared" si="17"/>
-        <v>39.800000000000011</v>
+        <f t="shared" si="16"/>
+        <v>40.866666666666674</v>
       </c>
       <c r="R14" s="7">
-        <f t="shared" si="17"/>
-        <v>38.400000000000013</v>
+        <f t="shared" si="16"/>
+        <v>39.600000000000009</v>
       </c>
       <c r="S14" s="7">
-        <f t="shared" si="17"/>
-        <v>37.000000000000014</v>
+        <f t="shared" si="16"/>
+        <v>38.333333333333343</v>
       </c>
       <c r="T14" s="7">
-        <f t="shared" si="17"/>
-        <v>35.600000000000016</v>
+        <f t="shared" si="16"/>
+        <v>37.066666666666677</v>
       </c>
       <c r="U14" s="7">
-        <f t="shared" si="17"/>
-        <v>34.200000000000017</v>
+        <f t="shared" si="16"/>
+        <v>35.800000000000011</v>
       </c>
       <c r="V14" s="7">
-        <f t="shared" si="17"/>
-        <v>32.800000000000018</v>
+        <f t="shared" si="16"/>
+        <v>34.533333333333346</v>
       </c>
       <c r="W14" s="7">
-        <f t="shared" si="17"/>
-        <v>31.40000000000002</v>
+        <f t="shared" si="16"/>
+        <v>33.26666666666668</v>
       </c>
       <c r="X14" s="7">
-        <f t="shared" si="17"/>
-        <v>30.000000000000021</v>
+        <f t="shared" si="16"/>
+        <v>32.000000000000014</v>
       </c>
       <c r="Y14" s="3">
         <v>13</v>
@@ -1765,87 +1796,87 @@
         <v>14</v>
       </c>
       <c r="D15" s="6">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="E15" s="6">
         <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="E15" s="6">
+        <v>21.333333333333343</v>
+      </c>
+      <c r="F15" s="6">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="F15" s="6">
-        <f t="shared" si="4"/>
-        <v>14</v>
+        <v>12.666666666666657</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>0.93333333333333335</v>
+        <f>-F15/(Width-1)</f>
+        <v>-0.84444444444444378</v>
       </c>
       <c r="H15" s="3">
         <v>14</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="J15" s="7">
-        <f t="shared" ref="J15:X15" si="18">I15-$G15</f>
-        <v>33.06666666666667</v>
+        <f t="shared" ref="J15:X15" si="17">I15+$G15</f>
+        <v>33.155555555555559</v>
       </c>
       <c r="K15" s="7">
-        <f t="shared" si="18"/>
-        <v>32.13333333333334</v>
+        <f t="shared" si="17"/>
+        <v>32.311111111111117</v>
       </c>
       <c r="L15" s="7">
-        <f t="shared" si="18"/>
-        <v>31.200000000000006</v>
+        <f t="shared" si="17"/>
+        <v>31.466666666666672</v>
       </c>
       <c r="M15" s="7">
-        <f t="shared" si="18"/>
-        <v>30.266666666666673</v>
+        <f t="shared" si="17"/>
+        <v>30.622222222222227</v>
       </c>
       <c r="N15" s="7">
-        <f t="shared" si="18"/>
-        <v>29.333333333333339</v>
+        <f t="shared" si="17"/>
+        <v>29.777777777777782</v>
       </c>
       <c r="O15" s="7">
-        <f t="shared" si="18"/>
-        <v>28.400000000000006</v>
+        <f t="shared" si="17"/>
+        <v>28.933333333333337</v>
       </c>
       <c r="P15" s="7">
-        <f t="shared" si="18"/>
-        <v>27.466666666666672</v>
+        <f t="shared" si="17"/>
+        <v>28.088888888888892</v>
       </c>
       <c r="Q15" s="7">
-        <f t="shared" si="18"/>
-        <v>26.533333333333339</v>
+        <f t="shared" si="17"/>
+        <v>27.244444444444447</v>
       </c>
       <c r="R15" s="7">
-        <f t="shared" si="18"/>
-        <v>25.600000000000005</v>
+        <f t="shared" si="17"/>
+        <v>26.400000000000002</v>
       </c>
       <c r="S15" s="7">
-        <f t="shared" si="18"/>
-        <v>24.666666666666671</v>
+        <f t="shared" si="17"/>
+        <v>25.555555555555557</v>
       </c>
       <c r="T15" s="7">
-        <f t="shared" si="18"/>
-        <v>23.733333333333338</v>
+        <f t="shared" si="17"/>
+        <v>24.711111111111112</v>
       </c>
       <c r="U15" s="7">
-        <f t="shared" si="18"/>
-        <v>22.800000000000004</v>
+        <f t="shared" si="17"/>
+        <v>23.866666666666667</v>
       </c>
       <c r="V15" s="7">
-        <f t="shared" si="18"/>
-        <v>21.866666666666671</v>
+        <f t="shared" si="17"/>
+        <v>23.022222222222222</v>
       </c>
       <c r="W15" s="7">
-        <f t="shared" si="18"/>
-        <v>20.933333333333337</v>
+        <f t="shared" si="17"/>
+        <v>22.177777777777777</v>
       </c>
       <c r="X15" s="7">
-        <f t="shared" si="18"/>
-        <v>20.000000000000004</v>
+        <f t="shared" si="17"/>
+        <v>21.333333333333332</v>
       </c>
       <c r="Y15" s="3">
         <v>14</v>
@@ -1856,87 +1887,87 @@
         <v>15</v>
       </c>
       <c r="D16" s="6">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="E16" s="6">
         <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="E16" s="6">
+        <v>10.666666666666677</v>
+      </c>
+      <c r="F16" s="6">
         <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="F16" s="6">
-        <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6.3333333333333233</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="0"/>
-        <v>0.46666666666666667</v>
+        <f>-F16/(Width-1)</f>
+        <v>-0.42222222222222155</v>
       </c>
       <c r="H16" s="3">
         <v>15</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" ref="J16:X16" si="19">I16-$G16</f>
-        <v>16.533333333333335</v>
+        <f t="shared" ref="J16:X16" si="18">I16+$G16</f>
+        <v>16.577777777777779</v>
       </c>
       <c r="K16" s="7">
-        <f t="shared" si="19"/>
-        <v>16.06666666666667</v>
+        <f t="shared" si="18"/>
+        <v>16.155555555555559</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" si="19"/>
-        <v>15.600000000000003</v>
+        <f t="shared" si="18"/>
+        <v>15.733333333333338</v>
       </c>
       <c r="M16" s="7">
-        <f t="shared" si="19"/>
-        <v>15.133333333333336</v>
+        <f t="shared" si="18"/>
+        <v>15.311111111111117</v>
       </c>
       <c r="N16" s="7">
-        <f t="shared" si="19"/>
-        <v>14.66666666666667</v>
+        <f t="shared" si="18"/>
+        <v>14.888888888888896</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="19"/>
-        <v>14.200000000000003</v>
+        <f t="shared" si="18"/>
+        <v>14.466666666666676</v>
       </c>
       <c r="P16" s="7">
-        <f t="shared" si="19"/>
-        <v>13.733333333333336</v>
+        <f t="shared" si="18"/>
+        <v>14.044444444444455</v>
       </c>
       <c r="Q16" s="7">
-        <f t="shared" si="19"/>
-        <v>13.266666666666669</v>
+        <f t="shared" si="18"/>
+        <v>13.622222222222234</v>
       </c>
       <c r="R16" s="7">
-        <f t="shared" si="19"/>
-        <v>12.800000000000002</v>
+        <f t="shared" si="18"/>
+        <v>13.200000000000014</v>
       </c>
       <c r="S16" s="7">
-        <f t="shared" si="19"/>
-        <v>12.333333333333336</v>
+        <f t="shared" si="18"/>
+        <v>12.777777777777793</v>
       </c>
       <c r="T16" s="7">
-        <f t="shared" si="19"/>
-        <v>11.866666666666669</v>
+        <f t="shared" si="18"/>
+        <v>12.355555555555572</v>
       </c>
       <c r="U16" s="7">
-        <f t="shared" si="19"/>
-        <v>11.400000000000002</v>
+        <f t="shared" si="18"/>
+        <v>11.933333333333351</v>
       </c>
       <c r="V16" s="7">
-        <f t="shared" si="19"/>
-        <v>10.933333333333335</v>
+        <f t="shared" si="18"/>
+        <v>11.511111111111131</v>
       </c>
       <c r="W16" s="7">
-        <f t="shared" si="19"/>
-        <v>10.466666666666669</v>
+        <f t="shared" si="18"/>
+        <v>11.08888888888891</v>
       </c>
       <c r="X16" s="7">
-        <f t="shared" si="19"/>
-        <v>10.000000000000002</v>
+        <f t="shared" si="18"/>
+        <v>10.666666666666689</v>
       </c>
       <c r="Y16" s="3">
         <v>15</v>
@@ -1947,86 +1978,86 @@
         <v>16</v>
       </c>
       <c r="D17" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F17" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="G17" s="6">
-        <f t="shared" si="0"/>
+        <f>-F17/(Width-1)</f>
         <v>0</v>
       </c>
       <c r="H17" s="3">
         <v>16</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" ref="J17:X17" si="20">I17-$G17</f>
+        <f t="shared" ref="J17:X17" si="19">I17+$G17</f>
         <v>0</v>
       </c>
       <c r="K17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="P17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="S17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="U17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X17" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y17" s="3">

</xml_diff>

<commit_message>
Color Control - Gradient capable
</commit_message>
<xml_diff>
--- a/doc/ColorPicker.xlsx
+++ b/doc/ColorPicker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ss\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DD8E46-234E-4D03-A110-96B210C168C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614CFE19-E40A-4C41-AFA5-19BDEE59343C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="4605" windowWidth="21585" windowHeight="15045" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
+    <workbookView xWindow="16920" yWindow="4605" windowWidth="21585" windowHeight="15045" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
   </bookViews>
   <sheets>
     <sheet name="Gradient" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -667,86 +667,86 @@
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D17" si="1">D2-VerticalStepL</f>
-        <v>238</v>
+        <v>239.33333333333334</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:E17" si="2">E2-VerticalStepR</f>
-        <v>149.33333333333334</v>
+        <v>152.66666666666666</v>
       </c>
       <c r="F3" s="6">
         <f t="shared" ref="F3:F17" si="3">D3-E3</f>
-        <v>88.666666666666657</v>
+        <v>86.666666666666686</v>
       </c>
       <c r="G3" s="6">
         <f>-F3/(Width-1)</f>
-        <v>-5.9111111111111105</v>
+        <v>-5.7777777777777795</v>
       </c>
       <c r="H3" s="3">
         <v>2</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" ref="I3:I17" si="4">D3</f>
-        <v>238</v>
+        <v>239.33333333333334</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" ref="J3:X3" si="5">I3+$G3</f>
-        <v>232.0888888888889</v>
+        <v>233.55555555555557</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="5"/>
-        <v>226.17777777777781</v>
+        <v>227.7777777777778</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="5"/>
-        <v>220.26666666666671</v>
+        <v>222.00000000000003</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="5"/>
-        <v>214.35555555555561</v>
+        <v>216.22222222222226</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" si="5"/>
-        <v>208.44444444444451</v>
+        <v>210.44444444444449</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="5"/>
-        <v>202.53333333333342</v>
+        <v>204.66666666666671</v>
       </c>
       <c r="P3" s="7">
         <f t="shared" si="5"/>
-        <v>196.62222222222232</v>
+        <v>198.88888888888894</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="5"/>
-        <v>190.71111111111122</v>
+        <v>193.11111111111117</v>
       </c>
       <c r="R3" s="7">
         <f t="shared" si="5"/>
-        <v>184.80000000000013</v>
+        <v>187.3333333333334</v>
       </c>
       <c r="S3" s="7">
         <f t="shared" si="5"/>
-        <v>178.88888888888903</v>
+        <v>181.55555555555563</v>
       </c>
       <c r="T3" s="7">
         <f t="shared" si="5"/>
-        <v>172.97777777777793</v>
+        <v>175.77777777777786</v>
       </c>
       <c r="U3" s="7">
         <f t="shared" si="5"/>
-        <v>167.06666666666683</v>
+        <v>170.00000000000009</v>
       </c>
       <c r="V3" s="7">
         <f t="shared" si="5"/>
-        <v>161.15555555555574</v>
+        <v>164.22222222222231</v>
       </c>
       <c r="W3" s="7">
         <f t="shared" si="5"/>
-        <v>155.24444444444464</v>
+        <v>158.44444444444454</v>
       </c>
       <c r="X3" s="7">
         <f t="shared" si="5"/>
-        <v>149.33333333333354</v>
+        <v>152.66666666666677</v>
       </c>
       <c r="Y3" s="3">
         <v>2</v>
@@ -757,93 +757,93 @@
         <v>10</v>
       </c>
       <c r="B4" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="1"/>
-        <v>221</v>
+        <v>223.66666666666669</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" si="2"/>
-        <v>138.66666666666669</v>
+        <v>145.33333333333331</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" si="3"/>
-        <v>82.333333333333314</v>
+        <v>78.333333333333371</v>
       </c>
       <c r="G4" s="6">
         <f>-F4/(Width-1)</f>
-        <v>-5.488888888888888</v>
+        <v>-5.222222222222225</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="4"/>
-        <v>221</v>
+        <v>223.66666666666669</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" ref="J4:X4" si="6">I4+$G4</f>
-        <v>215.51111111111112</v>
+        <v>218.44444444444446</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="6"/>
-        <v>210.02222222222224</v>
+        <v>213.22222222222223</v>
       </c>
       <c r="L4" s="7">
         <f t="shared" si="6"/>
-        <v>204.53333333333336</v>
+        <v>208</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" si="6"/>
-        <v>199.04444444444448</v>
+        <v>202.77777777777777</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" si="6"/>
-        <v>193.5555555555556</v>
+        <v>197.55555555555554</v>
       </c>
       <c r="O4" s="7">
         <f t="shared" si="6"/>
-        <v>188.06666666666672</v>
+        <v>192.33333333333331</v>
       </c>
       <c r="P4" s="7">
         <f t="shared" si="6"/>
-        <v>182.57777777777784</v>
+        <v>187.11111111111109</v>
       </c>
       <c r="Q4" s="7">
         <f t="shared" si="6"/>
-        <v>177.08888888888896</v>
+        <v>181.88888888888886</v>
       </c>
       <c r="R4" s="7">
         <f t="shared" si="6"/>
-        <v>171.60000000000008</v>
+        <v>176.66666666666663</v>
       </c>
       <c r="S4" s="7">
         <f t="shared" si="6"/>
-        <v>166.1111111111112</v>
+        <v>171.4444444444444</v>
       </c>
       <c r="T4" s="7">
         <f t="shared" si="6"/>
-        <v>160.62222222222232</v>
+        <v>166.22222222222217</v>
       </c>
       <c r="U4" s="7">
         <f t="shared" si="6"/>
-        <v>155.13333333333344</v>
+        <v>160.99999999999994</v>
       </c>
       <c r="V4" s="7">
         <f t="shared" si="6"/>
-        <v>149.64444444444456</v>
+        <v>155.77777777777771</v>
       </c>
       <c r="W4" s="7">
         <f t="shared" si="6"/>
-        <v>144.15555555555568</v>
+        <v>150.55555555555549</v>
       </c>
       <c r="X4" s="7">
         <f t="shared" si="6"/>
-        <v>138.6666666666668</v>
+        <v>145.33333333333326</v>
       </c>
       <c r="Y4" s="3">
         <v>3</v>
@@ -854,93 +854,93 @@
         <v>11</v>
       </c>
       <c r="B5" s="8">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="1"/>
-        <v>204</v>
+        <v>208.00000000000003</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="2"/>
-        <v>128.00000000000003</v>
+        <v>137.99999999999997</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="3"/>
-        <v>75.999999999999972</v>
+        <v>70.000000000000057</v>
       </c>
       <c r="G5" s="6">
         <f>-F5/(Width-1)</f>
-        <v>-5.0666666666666647</v>
+        <v>-4.6666666666666705</v>
       </c>
       <c r="H5" s="3">
         <v>4</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="4"/>
-        <v>204</v>
+        <v>208.00000000000003</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" ref="J5:X5" si="7">I5+$G5</f>
-        <v>198.93333333333334</v>
+        <v>203.33333333333337</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="7"/>
-        <v>193.86666666666667</v>
+        <v>198.66666666666671</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="7"/>
-        <v>188.8</v>
+        <v>194.00000000000006</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="7"/>
-        <v>183.73333333333335</v>
+        <v>189.3333333333334</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="7"/>
-        <v>178.66666666666669</v>
+        <v>184.66666666666674</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="7"/>
-        <v>173.60000000000002</v>
+        <v>180.00000000000009</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="7"/>
-        <v>168.53333333333336</v>
+        <v>175.33333333333343</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="7"/>
-        <v>163.4666666666667</v>
+        <v>170.66666666666677</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="7"/>
-        <v>158.40000000000003</v>
+        <v>166.00000000000011</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="7"/>
-        <v>153.33333333333337</v>
+        <v>161.33333333333346</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="7"/>
-        <v>148.26666666666671</v>
+        <v>156.6666666666668</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="7"/>
-        <v>143.20000000000005</v>
+        <v>152.00000000000014</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="7"/>
-        <v>138.13333333333338</v>
+        <v>147.33333333333348</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="7"/>
-        <v>133.06666666666672</v>
+        <v>142.66666666666683</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" si="7"/>
-        <v>128.00000000000006</v>
+        <v>138.00000000000017</v>
       </c>
       <c r="Y5" s="3">
         <v>4</v>
@@ -958,86 +958,86 @@
       </c>
       <c r="D6" s="6">
         <f t="shared" si="1"/>
-        <v>187</v>
+        <v>192.33333333333337</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="2"/>
-        <v>117.33333333333336</v>
+        <v>130.66666666666663</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="3"/>
-        <v>69.666666666666643</v>
+        <v>61.666666666666742</v>
       </c>
       <c r="G6" s="6">
         <f>-F6/(Width-1)</f>
-        <v>-4.644444444444443</v>
+        <v>-4.111111111111116</v>
       </c>
       <c r="H6" s="3">
         <v>5</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="4"/>
-        <v>187</v>
+        <v>192.33333333333337</v>
       </c>
       <c r="J6" s="7">
         <f t="shared" ref="J6:X6" si="8">I6+$G6</f>
-        <v>182.35555555555555</v>
+        <v>188.22222222222226</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="8"/>
-        <v>177.71111111111111</v>
+        <v>184.11111111111114</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" si="8"/>
-        <v>173.06666666666666</v>
+        <v>180.00000000000003</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" si="8"/>
-        <v>168.42222222222222</v>
+        <v>175.88888888888891</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="8"/>
-        <v>163.77777777777777</v>
+        <v>171.7777777777778</v>
       </c>
       <c r="O6" s="7">
         <f t="shared" si="8"/>
-        <v>159.13333333333333</v>
+        <v>167.66666666666669</v>
       </c>
       <c r="P6" s="7">
         <f t="shared" si="8"/>
-        <v>154.48888888888888</v>
+        <v>163.55555555555557</v>
       </c>
       <c r="Q6" s="7">
         <f t="shared" si="8"/>
-        <v>149.84444444444443</v>
+        <v>159.44444444444446</v>
       </c>
       <c r="R6" s="7">
         <f t="shared" si="8"/>
-        <v>145.19999999999999</v>
+        <v>155.33333333333334</v>
       </c>
       <c r="S6" s="7">
         <f t="shared" si="8"/>
-        <v>140.55555555555554</v>
+        <v>151.22222222222223</v>
       </c>
       <c r="T6" s="7">
         <f t="shared" si="8"/>
-        <v>135.9111111111111</v>
+        <v>147.11111111111111</v>
       </c>
       <c r="U6" s="7">
         <f t="shared" si="8"/>
-        <v>131.26666666666665</v>
+        <v>143</v>
       </c>
       <c r="V6" s="7">
         <f t="shared" si="8"/>
-        <v>126.62222222222221</v>
+        <v>138.88888888888889</v>
       </c>
       <c r="W6" s="7">
         <f t="shared" si="8"/>
-        <v>121.97777777777776</v>
+        <v>134.77777777777777</v>
       </c>
       <c r="X6" s="7">
         <f t="shared" si="8"/>
-        <v>117.33333333333331</v>
+        <v>130.66666666666666</v>
       </c>
       <c r="Y6" s="3">
         <v>5</v>
@@ -1055,86 +1055,86 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" si="1"/>
-        <v>170</v>
+        <v>176.66666666666671</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="2"/>
-        <v>106.66666666666669</v>
+        <v>123.3333333333333</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="3"/>
-        <v>63.333333333333314</v>
+        <v>53.333333333333414</v>
       </c>
       <c r="G7" s="6">
         <f>-F7/(Width-1)</f>
-        <v>-4.2222222222222205</v>
+        <v>-3.5555555555555611</v>
       </c>
       <c r="H7" s="3">
         <v>6</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="4"/>
-        <v>170</v>
+        <v>176.66666666666671</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" ref="J7:X7" si="9">I7+$G7</f>
-        <v>165.77777777777777</v>
+        <v>173.11111111111114</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="9"/>
-        <v>161.55555555555554</v>
+        <v>169.55555555555557</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="9"/>
-        <v>157.33333333333331</v>
+        <v>166</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="9"/>
-        <v>153.11111111111109</v>
+        <v>162.44444444444443</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="9"/>
-        <v>148.88888888888886</v>
+        <v>158.88888888888886</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="9"/>
-        <v>144.66666666666663</v>
+        <v>155.33333333333329</v>
       </c>
       <c r="P7" s="7">
         <f t="shared" si="9"/>
-        <v>140.4444444444444</v>
+        <v>151.77777777777771</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="9"/>
-        <v>136.22222222222217</v>
+        <v>148.22222222222214</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="9"/>
-        <v>131.99999999999994</v>
+        <v>144.66666666666657</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="9"/>
-        <v>127.77777777777773</v>
+        <v>141.111111111111</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="9"/>
-        <v>123.55555555555551</v>
+        <v>137.55555555555543</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="9"/>
-        <v>119.3333333333333</v>
+        <v>133.99999999999986</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="9"/>
-        <v>115.11111111111109</v>
+        <v>130.44444444444429</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="9"/>
-        <v>110.88888888888887</v>
+        <v>126.88888888888873</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="9"/>
-        <v>106.66666666666666</v>
+        <v>123.33333333333317</v>
       </c>
       <c r="Y7" s="3">
         <v>6</v>
@@ -1146,93 +1146,93 @@
       </c>
       <c r="B8" s="6">
         <f>(TopLeft-BottomLeft)/(Height-1)</f>
-        <v>17</v>
+        <v>15.666666666666666</v>
       </c>
       <c r="C8" s="3">
         <v>7</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="1"/>
-        <v>153</v>
+        <v>161.00000000000006</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="2"/>
-        <v>96.000000000000014</v>
+        <v>115.99999999999997</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" si="3"/>
-        <v>56.999999999999986</v>
+        <v>45.000000000000085</v>
       </c>
       <c r="G8" s="6">
         <f>-F8/(Width-1)</f>
-        <v>-3.7999999999999989</v>
+        <v>-3.0000000000000058</v>
       </c>
       <c r="H8" s="3">
         <v>7</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="4"/>
-        <v>153</v>
+        <v>161.00000000000006</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" ref="J8:X8" si="10">I8+$G8</f>
-        <v>149.19999999999999</v>
+        <v>158.00000000000006</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="10"/>
-        <v>145.39999999999998</v>
+        <v>155.00000000000006</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" si="10"/>
-        <v>141.59999999999997</v>
+        <v>152.00000000000006</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="10"/>
-        <v>137.79999999999995</v>
+        <v>149.00000000000006</v>
       </c>
       <c r="N8" s="7">
         <f t="shared" si="10"/>
-        <v>133.99999999999994</v>
+        <v>146.00000000000006</v>
       </c>
       <c r="O8" s="7">
         <f t="shared" si="10"/>
-        <v>130.19999999999993</v>
+        <v>143.00000000000006</v>
       </c>
       <c r="P8" s="7">
         <f t="shared" si="10"/>
-        <v>126.39999999999993</v>
+        <v>140.00000000000006</v>
       </c>
       <c r="Q8" s="7">
         <f t="shared" si="10"/>
-        <v>122.59999999999994</v>
+        <v>137.00000000000006</v>
       </c>
       <c r="R8" s="7">
         <f t="shared" si="10"/>
-        <v>118.79999999999994</v>
+        <v>134.00000000000006</v>
       </c>
       <c r="S8" s="7">
         <f t="shared" si="10"/>
-        <v>114.99999999999994</v>
+        <v>131.00000000000006</v>
       </c>
       <c r="T8" s="7">
         <f t="shared" si="10"/>
-        <v>111.19999999999995</v>
+        <v>128.00000000000006</v>
       </c>
       <c r="U8" s="7">
         <f t="shared" si="10"/>
-        <v>107.39999999999995</v>
+        <v>125.00000000000006</v>
       </c>
       <c r="V8" s="7">
         <f t="shared" si="10"/>
-        <v>103.59999999999995</v>
+        <v>122.00000000000006</v>
       </c>
       <c r="W8" s="7">
         <f t="shared" si="10"/>
-        <v>99.799999999999955</v>
+        <v>119.00000000000006</v>
       </c>
       <c r="X8" s="7">
         <f t="shared" si="10"/>
-        <v>95.999999999999957</v>
+        <v>116.00000000000006</v>
       </c>
       <c r="Y8" s="3">
         <v>7</v>
@@ -1244,93 +1244,93 @@
       </c>
       <c r="B9" s="1">
         <f>(TopRight-BottomRight)/(Height - 1)</f>
-        <v>10.666666666666666</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>145.3333333333334</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="2"/>
-        <v>85.333333333333343</v>
+        <v>108.66666666666664</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="3"/>
-        <v>50.666666666666657</v>
+        <v>36.666666666666757</v>
       </c>
       <c r="G9" s="6">
         <f>-F9/(Width-1)</f>
-        <v>-3.3777777777777773</v>
+        <v>-2.4444444444444504</v>
       </c>
       <c r="H9" s="3">
         <v>8</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="4"/>
-        <v>136</v>
+        <v>145.3333333333334</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" ref="J9:X9" si="11">I9+$G9</f>
-        <v>132.62222222222223</v>
+        <v>142.88888888888894</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="11"/>
-        <v>129.24444444444447</v>
+        <v>140.44444444444449</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="11"/>
-        <v>125.86666666666669</v>
+        <v>138.00000000000003</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="11"/>
-        <v>122.48888888888891</v>
+        <v>135.55555555555557</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="11"/>
-        <v>119.11111111111113</v>
+        <v>133.11111111111111</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="11"/>
-        <v>115.73333333333335</v>
+        <v>130.66666666666666</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="11"/>
-        <v>112.35555555555557</v>
+        <v>128.2222222222222</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="11"/>
-        <v>108.97777777777779</v>
+        <v>125.77777777777774</v>
       </c>
       <c r="R9" s="7">
         <f t="shared" si="11"/>
-        <v>105.60000000000001</v>
+        <v>123.33333333333329</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="11"/>
-        <v>102.22222222222223</v>
+        <v>120.88888888888883</v>
       </c>
       <c r="T9" s="7">
         <f t="shared" si="11"/>
-        <v>98.844444444444449</v>
+        <v>118.44444444444437</v>
       </c>
       <c r="U9" s="7">
         <f t="shared" si="11"/>
-        <v>95.466666666666669</v>
+        <v>115.99999999999991</v>
       </c>
       <c r="V9" s="7">
         <f t="shared" si="11"/>
-        <v>92.088888888888889</v>
+        <v>113.55555555555546</v>
       </c>
       <c r="W9" s="7">
         <f t="shared" si="11"/>
-        <v>88.711111111111109</v>
+        <v>111.111111111111</v>
       </c>
       <c r="X9" s="7">
         <f t="shared" si="11"/>
-        <v>85.333333333333329</v>
+        <v>108.66666666666654</v>
       </c>
       <c r="Y9" s="3">
         <v>8</v>
@@ -1342,86 +1342,86 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>129.66666666666674</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="2"/>
-        <v>74.666666666666671</v>
+        <v>101.33333333333331</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="3"/>
-        <v>44.333333333333329</v>
+        <v>28.333333333333428</v>
       </c>
       <c r="G10" s="6">
         <f>-F10/(Width-1)</f>
-        <v>-2.9555555555555553</v>
+        <v>-1.8888888888888953</v>
       </c>
       <c r="H10" s="3">
         <v>9</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="4"/>
-        <v>119</v>
+        <v>129.66666666666674</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" ref="J10:X10" si="12">I10+$G10</f>
-        <v>116.04444444444445</v>
+        <v>127.77777777777784</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="12"/>
-        <v>113.0888888888889</v>
+        <v>125.88888888888894</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="12"/>
-        <v>110.13333333333335</v>
+        <v>124.00000000000004</v>
       </c>
       <c r="M10" s="7">
         <f t="shared" si="12"/>
-        <v>107.17777777777781</v>
+        <v>122.11111111111114</v>
       </c>
       <c r="N10" s="7">
         <f t="shared" si="12"/>
-        <v>104.22222222222226</v>
+        <v>120.22222222222224</v>
       </c>
       <c r="O10" s="7">
         <f t="shared" si="12"/>
-        <v>101.26666666666671</v>
+        <v>118.33333333333334</v>
       </c>
       <c r="P10" s="7">
         <f t="shared" si="12"/>
-        <v>98.31111111111116</v>
+        <v>116.44444444444444</v>
       </c>
       <c r="Q10" s="7">
         <f t="shared" si="12"/>
-        <v>95.355555555555611</v>
+        <v>114.55555555555554</v>
       </c>
       <c r="R10" s="7">
         <f t="shared" si="12"/>
-        <v>92.400000000000063</v>
+        <v>112.66666666666664</v>
       </c>
       <c r="S10" s="7">
         <f t="shared" si="12"/>
-        <v>89.444444444444514</v>
+        <v>110.77777777777774</v>
       </c>
       <c r="T10" s="7">
         <f t="shared" si="12"/>
-        <v>86.488888888888965</v>
+        <v>108.88888888888884</v>
       </c>
       <c r="U10" s="7">
         <f t="shared" si="12"/>
-        <v>83.533333333333417</v>
+        <v>106.99999999999994</v>
       </c>
       <c r="V10" s="7">
         <f t="shared" si="12"/>
-        <v>80.577777777777868</v>
+        <v>105.11111111111104</v>
       </c>
       <c r="W10" s="7">
         <f t="shared" si="12"/>
-        <v>77.622222222222319</v>
+        <v>103.22222222222214</v>
       </c>
       <c r="X10" s="7">
         <f t="shared" si="12"/>
-        <v>74.666666666666771</v>
+        <v>101.33333333333324</v>
       </c>
       <c r="Y10" s="3">
         <v>9</v>
@@ -1433,86 +1433,86 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>114.00000000000007</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>93.999999999999986</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>20.000000000000085</v>
       </c>
       <c r="G11" s="6">
         <f>-F11/(Width-1)</f>
-        <v>-2.5333333333333332</v>
+        <v>-1.333333333333339</v>
       </c>
       <c r="H11" s="3">
         <v>10</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="4"/>
-        <v>102</v>
+        <v>114.00000000000007</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" ref="J11:X11" si="13">I11+$G11</f>
-        <v>99.466666666666669</v>
+        <v>112.66666666666673</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="13"/>
-        <v>96.933333333333337</v>
+        <v>111.33333333333339</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="13"/>
-        <v>94.4</v>
+        <v>110.00000000000004</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="13"/>
-        <v>91.866666666666674</v>
+        <v>108.6666666666667</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" si="13"/>
-        <v>89.333333333333343</v>
+        <v>107.33333333333336</v>
       </c>
       <c r="O11" s="7">
         <f t="shared" si="13"/>
-        <v>86.800000000000011</v>
+        <v>106.00000000000001</v>
       </c>
       <c r="P11" s="7">
         <f t="shared" si="13"/>
-        <v>84.26666666666668</v>
+        <v>104.66666666666667</v>
       </c>
       <c r="Q11" s="7">
         <f t="shared" si="13"/>
-        <v>81.733333333333348</v>
+        <v>103.33333333333333</v>
       </c>
       <c r="R11" s="7">
         <f t="shared" si="13"/>
-        <v>79.200000000000017</v>
+        <v>101.99999999999999</v>
       </c>
       <c r="S11" s="7">
         <f t="shared" si="13"/>
-        <v>76.666666666666686</v>
+        <v>100.66666666666664</v>
       </c>
       <c r="T11" s="7">
         <f t="shared" si="13"/>
-        <v>74.133333333333354</v>
+        <v>99.3333333333333</v>
       </c>
       <c r="U11" s="7">
         <f t="shared" si="13"/>
-        <v>71.600000000000023</v>
+        <v>97.999999999999957</v>
       </c>
       <c r="V11" s="7">
         <f t="shared" si="13"/>
-        <v>69.066666666666691</v>
+        <v>96.666666666666615</v>
       </c>
       <c r="W11" s="7">
         <f t="shared" si="13"/>
-        <v>66.53333333333336</v>
+        <v>95.333333333333272</v>
       </c>
       <c r="X11" s="7">
         <f t="shared" si="13"/>
-        <v>64.000000000000028</v>
+        <v>93.999999999999929</v>
       </c>
       <c r="Y11" s="3">
         <v>10</v>
@@ -1524,86 +1524,86 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>98.3333333333334</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="2"/>
-        <v>53.333333333333336</v>
+        <v>86.666666666666657</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="3"/>
-        <v>31.666666666666664</v>
+        <v>11.666666666666742</v>
       </c>
       <c r="G12" s="6">
         <f>-F12/(Width-1)</f>
-        <v>-2.1111111111111112</v>
+        <v>-0.77777777777778279</v>
       </c>
       <c r="H12" s="3">
         <v>11</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="4"/>
-        <v>85</v>
+        <v>98.3333333333334</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" ref="J12:X12" si="14">I12+$G12</f>
-        <v>82.888888888888886</v>
+        <v>97.555555555555614</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="14"/>
-        <v>80.777777777777771</v>
+        <v>96.777777777777828</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" si="14"/>
-        <v>78.666666666666657</v>
+        <v>96.000000000000043</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" si="14"/>
-        <v>76.555555555555543</v>
+        <v>95.222222222222257</v>
       </c>
       <c r="N12" s="7">
         <f t="shared" si="14"/>
-        <v>74.444444444444429</v>
+        <v>94.444444444444471</v>
       </c>
       <c r="O12" s="7">
         <f t="shared" si="14"/>
-        <v>72.333333333333314</v>
+        <v>93.666666666666686</v>
       </c>
       <c r="P12" s="7">
         <f t="shared" si="14"/>
-        <v>70.2222222222222</v>
+        <v>92.8888888888889</v>
       </c>
       <c r="Q12" s="7">
         <f t="shared" si="14"/>
-        <v>68.111111111111086</v>
+        <v>92.111111111111114</v>
       </c>
       <c r="R12" s="7">
         <f t="shared" si="14"/>
-        <v>65.999999999999972</v>
+        <v>91.333333333333329</v>
       </c>
       <c r="S12" s="7">
         <f t="shared" si="14"/>
-        <v>63.888888888888857</v>
+        <v>90.555555555555543</v>
       </c>
       <c r="T12" s="7">
         <f t="shared" si="14"/>
-        <v>61.777777777777743</v>
+        <v>89.777777777777757</v>
       </c>
       <c r="U12" s="7">
         <f t="shared" si="14"/>
-        <v>59.666666666666629</v>
+        <v>88.999999999999972</v>
       </c>
       <c r="V12" s="7">
         <f t="shared" si="14"/>
-        <v>57.555555555555515</v>
+        <v>88.222222222222186</v>
       </c>
       <c r="W12" s="7">
         <f t="shared" si="14"/>
-        <v>55.4444444444444</v>
+        <v>87.4444444444444</v>
       </c>
       <c r="X12" s="7">
         <f t="shared" si="14"/>
-        <v>53.333333333333286</v>
+        <v>86.666666666666615</v>
       </c>
       <c r="Y12" s="3">
         <v>11</v>
@@ -1615,86 +1615,86 @@
       </c>
       <c r="D13" s="6">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>82.666666666666728</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="2"/>
-        <v>42.666666666666671</v>
+        <v>79.333333333333329</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" si="3"/>
-        <v>25.333333333333329</v>
+        <v>3.3333333333333997</v>
       </c>
       <c r="G13" s="6">
         <f>-F13/(Width-1)</f>
-        <v>-1.6888888888888887</v>
+        <v>-0.22222222222222665</v>
       </c>
       <c r="H13" s="3">
         <v>12</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>82.666666666666728</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" ref="J13:X13" si="15">I13+$G13</f>
-        <v>66.311111111111117</v>
+        <v>82.4444444444445</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="15"/>
-        <v>64.622222222222234</v>
+        <v>82.222222222222271</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" si="15"/>
-        <v>62.933333333333344</v>
+        <v>82.000000000000043</v>
       </c>
       <c r="M13" s="7">
         <f t="shared" si="15"/>
-        <v>61.244444444444454</v>
+        <v>81.777777777777814</v>
       </c>
       <c r="N13" s="7">
         <f t="shared" si="15"/>
-        <v>59.555555555555564</v>
+        <v>81.555555555555586</v>
       </c>
       <c r="O13" s="7">
         <f t="shared" si="15"/>
-        <v>57.866666666666674</v>
+        <v>81.333333333333357</v>
       </c>
       <c r="P13" s="7">
         <f t="shared" si="15"/>
-        <v>56.177777777777784</v>
+        <v>81.111111111111128</v>
       </c>
       <c r="Q13" s="7">
         <f t="shared" si="15"/>
-        <v>54.488888888888894</v>
+        <v>80.8888888888889</v>
       </c>
       <c r="R13" s="7">
         <f t="shared" si="15"/>
-        <v>52.800000000000004</v>
+        <v>80.666666666666671</v>
       </c>
       <c r="S13" s="7">
         <f t="shared" si="15"/>
-        <v>51.111111111111114</v>
+        <v>80.444444444444443</v>
       </c>
       <c r="T13" s="7">
         <f t="shared" si="15"/>
-        <v>49.422222222222224</v>
+        <v>80.222222222222214</v>
       </c>
       <c r="U13" s="7">
         <f t="shared" si="15"/>
-        <v>47.733333333333334</v>
+        <v>79.999999999999986</v>
       </c>
       <c r="V13" s="7">
         <f t="shared" si="15"/>
-        <v>46.044444444444444</v>
+        <v>79.777777777777757</v>
       </c>
       <c r="W13" s="7">
         <f t="shared" si="15"/>
-        <v>44.355555555555554</v>
+        <v>79.555555555555529</v>
       </c>
       <c r="X13" s="7">
         <f t="shared" si="15"/>
-        <v>42.666666666666664</v>
+        <v>79.3333333333333</v>
       </c>
       <c r="Y13" s="3">
         <v>12</v>
@@ -1706,86 +1706,86 @@
       </c>
       <c r="D14" s="6">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>67.000000000000057</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" si="2"/>
-        <v>32.000000000000007</v>
+        <v>72</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" si="3"/>
-        <v>18.999999999999993</v>
+        <v>-4.9999999999999432</v>
       </c>
       <c r="G14" s="6">
         <f>-F14/(Width-1)</f>
-        <v>-1.2666666666666662</v>
+        <v>0.33333333333332954</v>
       </c>
       <c r="H14" s="3">
         <v>13</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>67.000000000000057</v>
       </c>
       <c r="J14" s="7">
         <f t="shared" ref="J14:X14" si="16">I14+$G14</f>
-        <v>49.733333333333334</v>
+        <v>67.333333333333385</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="16"/>
-        <v>48.466666666666669</v>
+        <v>67.666666666666714</v>
       </c>
       <c r="L14" s="7">
         <f t="shared" si="16"/>
-        <v>47.2</v>
+        <v>68.000000000000043</v>
       </c>
       <c r="M14" s="7">
         <f t="shared" si="16"/>
-        <v>45.933333333333337</v>
+        <v>68.333333333333371</v>
       </c>
       <c r="N14" s="7">
         <f t="shared" si="16"/>
-        <v>44.666666666666671</v>
+        <v>68.6666666666667</v>
       </c>
       <c r="O14" s="7">
         <f t="shared" si="16"/>
-        <v>43.400000000000006</v>
+        <v>69.000000000000028</v>
       </c>
       <c r="P14" s="7">
         <f t="shared" si="16"/>
-        <v>42.13333333333334</v>
+        <v>69.333333333333357</v>
       </c>
       <c r="Q14" s="7">
         <f t="shared" si="16"/>
-        <v>40.866666666666674</v>
+        <v>69.666666666666686</v>
       </c>
       <c r="R14" s="7">
         <f t="shared" si="16"/>
-        <v>39.600000000000009</v>
+        <v>70.000000000000014</v>
       </c>
       <c r="S14" s="7">
         <f t="shared" si="16"/>
-        <v>38.333333333333343</v>
+        <v>70.333333333333343</v>
       </c>
       <c r="T14" s="7">
         <f t="shared" si="16"/>
-        <v>37.066666666666677</v>
+        <v>70.666666666666671</v>
       </c>
       <c r="U14" s="7">
         <f t="shared" si="16"/>
-        <v>35.800000000000011</v>
+        <v>71</v>
       </c>
       <c r="V14" s="7">
         <f t="shared" si="16"/>
-        <v>34.533333333333346</v>
+        <v>71.333333333333329</v>
       </c>
       <c r="W14" s="7">
         <f t="shared" si="16"/>
-        <v>33.26666666666668</v>
+        <v>71.666666666666657</v>
       </c>
       <c r="X14" s="7">
         <f t="shared" si="16"/>
-        <v>32.000000000000014</v>
+        <v>71.999999999999986</v>
       </c>
       <c r="Y14" s="3">
         <v>13</v>
@@ -1797,86 +1797,86 @@
       </c>
       <c r="D15" s="6">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>51.333333333333393</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="2"/>
-        <v>21.333333333333343</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" si="3"/>
-        <v>12.666666666666657</v>
+        <v>-13.333333333333279</v>
       </c>
       <c r="G15" s="6">
         <f>-F15/(Width-1)</f>
-        <v>-0.84444444444444378</v>
+        <v>0.88888888888888529</v>
       </c>
       <c r="H15" s="3">
         <v>14</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>51.333333333333393</v>
       </c>
       <c r="J15" s="7">
         <f t="shared" ref="J15:X15" si="17">I15+$G15</f>
-        <v>33.155555555555559</v>
+        <v>52.222222222222278</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="17"/>
-        <v>32.311111111111117</v>
+        <v>53.111111111111164</v>
       </c>
       <c r="L15" s="7">
         <f t="shared" si="17"/>
-        <v>31.466666666666672</v>
+        <v>54.00000000000005</v>
       </c>
       <c r="M15" s="7">
         <f t="shared" si="17"/>
-        <v>30.622222222222227</v>
+        <v>54.888888888888935</v>
       </c>
       <c r="N15" s="7">
         <f t="shared" si="17"/>
-        <v>29.777777777777782</v>
+        <v>55.777777777777821</v>
       </c>
       <c r="O15" s="7">
         <f t="shared" si="17"/>
-        <v>28.933333333333337</v>
+        <v>56.666666666666707</v>
       </c>
       <c r="P15" s="7">
         <f t="shared" si="17"/>
-        <v>28.088888888888892</v>
+        <v>57.555555555555593</v>
       </c>
       <c r="Q15" s="7">
         <f t="shared" si="17"/>
-        <v>27.244444444444447</v>
+        <v>58.444444444444478</v>
       </c>
       <c r="R15" s="7">
         <f t="shared" si="17"/>
-        <v>26.400000000000002</v>
+        <v>59.333333333333364</v>
       </c>
       <c r="S15" s="7">
         <f t="shared" si="17"/>
-        <v>25.555555555555557</v>
+        <v>60.22222222222225</v>
       </c>
       <c r="T15" s="7">
         <f t="shared" si="17"/>
-        <v>24.711111111111112</v>
+        <v>61.111111111111136</v>
       </c>
       <c r="U15" s="7">
         <f t="shared" si="17"/>
-        <v>23.866666666666667</v>
+        <v>62.000000000000021</v>
       </c>
       <c r="V15" s="7">
         <f t="shared" si="17"/>
-        <v>23.022222222222222</v>
+        <v>62.888888888888907</v>
       </c>
       <c r="W15" s="7">
         <f t="shared" si="17"/>
-        <v>22.177777777777777</v>
+        <v>63.777777777777793</v>
       </c>
       <c r="X15" s="7">
         <f t="shared" si="17"/>
-        <v>21.333333333333332</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Y15" s="3">
         <v>14</v>
@@ -1888,86 +1888,86 @@
       </c>
       <c r="D16" s="6">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>35.666666666666728</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" si="2"/>
-        <v>10.666666666666677</v>
+        <v>57.333333333333336</v>
       </c>
       <c r="F16" s="6">
         <f t="shared" si="3"/>
-        <v>6.3333333333333233</v>
+        <v>-21.666666666666607</v>
       </c>
       <c r="G16" s="6">
         <f>-F16/(Width-1)</f>
-        <v>-0.42222222222222155</v>
+        <v>1.4444444444444404</v>
       </c>
       <c r="H16" s="3">
         <v>15</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>35.666666666666728</v>
       </c>
       <c r="J16" s="7">
         <f t="shared" ref="J16:X16" si="18">I16+$G16</f>
-        <v>16.577777777777779</v>
+        <v>37.111111111111171</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="18"/>
-        <v>16.155555555555559</v>
+        <v>38.555555555555614</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="18"/>
-        <v>15.733333333333338</v>
+        <v>40.000000000000057</v>
       </c>
       <c r="M16" s="7">
         <f t="shared" si="18"/>
-        <v>15.311111111111117</v>
+        <v>41.4444444444445</v>
       </c>
       <c r="N16" s="7">
         <f t="shared" si="18"/>
-        <v>14.888888888888896</v>
+        <v>42.888888888888943</v>
       </c>
       <c r="O16" s="7">
         <f t="shared" si="18"/>
-        <v>14.466666666666676</v>
+        <v>44.333333333333385</v>
       </c>
       <c r="P16" s="7">
         <f t="shared" si="18"/>
-        <v>14.044444444444455</v>
+        <v>45.777777777777828</v>
       </c>
       <c r="Q16" s="7">
         <f t="shared" si="18"/>
-        <v>13.622222222222234</v>
+        <v>47.222222222222271</v>
       </c>
       <c r="R16" s="7">
         <f t="shared" si="18"/>
-        <v>13.200000000000014</v>
+        <v>48.666666666666714</v>
       </c>
       <c r="S16" s="7">
         <f t="shared" si="18"/>
-        <v>12.777777777777793</v>
+        <v>50.111111111111157</v>
       </c>
       <c r="T16" s="7">
         <f t="shared" si="18"/>
-        <v>12.355555555555572</v>
+        <v>51.5555555555556</v>
       </c>
       <c r="U16" s="7">
         <f t="shared" si="18"/>
-        <v>11.933333333333351</v>
+        <v>53.000000000000043</v>
       </c>
       <c r="V16" s="7">
         <f t="shared" si="18"/>
-        <v>11.511111111111131</v>
+        <v>54.444444444444485</v>
       </c>
       <c r="W16" s="7">
         <f t="shared" si="18"/>
-        <v>11.08888888888891</v>
+        <v>55.888888888888928</v>
       </c>
       <c r="X16" s="7">
         <f t="shared" si="18"/>
-        <v>10.666666666666689</v>
+        <v>57.333333333333371</v>
       </c>
       <c r="Y16" s="3">
         <v>15</v>
@@ -1979,86 +1979,86 @@
       </c>
       <c r="D17" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20.000000000000064</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F17" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-29.999999999999936</v>
       </c>
       <c r="G17" s="6">
         <f>-F17/(Width-1)</f>
-        <v>0</v>
+        <v>1.9999999999999958</v>
       </c>
       <c r="H17" s="3">
         <v>16</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>20.000000000000064</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" ref="J17:X17" si="19">I17+$G17</f>
-        <v>0</v>
+        <v>22.00000000000006</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>24.000000000000057</v>
       </c>
       <c r="L17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>26.000000000000053</v>
       </c>
       <c r="M17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>28.00000000000005</v>
       </c>
       <c r="N17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>30.000000000000046</v>
       </c>
       <c r="O17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>32.000000000000043</v>
       </c>
       <c r="P17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>34.000000000000036</v>
       </c>
       <c r="Q17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>36.000000000000028</v>
       </c>
       <c r="R17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>38.000000000000021</v>
       </c>
       <c r="S17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>40.000000000000014</v>
       </c>
       <c r="T17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>42.000000000000007</v>
       </c>
       <c r="U17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="V17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>45.999999999999993</v>
       </c>
       <c r="W17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>47.999999999999986</v>
       </c>
       <c r="X17" s="7">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>49.999999999999979</v>
       </c>
       <c r="Y17" s="3">
         <v>16</v>

</xml_diff>

<commit_message>
Gradient Bar - WIP
</commit_message>
<xml_diff>
--- a/doc/ColorPicker.xlsx
+++ b/doc/ColorPicker.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ss\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614CFE19-E40A-4C41-AFA5-19BDEE59343C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3038C6A4-ED0C-426E-AB64-4DE1EA790F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="4605" windowWidth="21585" windowHeight="15045" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
+    <workbookView xWindow="12675" yWindow="2505" windowWidth="21180" windowHeight="15090" activeTab="1" xr2:uid="{6F1C118E-D4F5-4070-9449-0D479C13C246}"/>
   </bookViews>
   <sheets>
-    <sheet name="Gradient" sheetId="1" r:id="rId1"/>
+    <sheet name="GradientMap" sheetId="1" r:id="rId1"/>
+    <sheet name="GradientBar" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="BottomLeft">Gradient!$B$4</definedName>
-    <definedName name="BottomRight">Gradient!$B$5</definedName>
-    <definedName name="Height">Gradient!$B$7</definedName>
-    <definedName name="TopLeft">Gradient!$B$2</definedName>
-    <definedName name="TopRight">Gradient!$B$3</definedName>
-    <definedName name="VerticalStepL">Gradient!$B$8</definedName>
-    <definedName name="VerticalStepR">Gradient!$B$9</definedName>
-    <definedName name="Width">Gradient!$B$6</definedName>
+    <definedName name="BarHeight">GradientBar!$B$3</definedName>
+    <definedName name="BarStep">GradientBar!$B$4</definedName>
+    <definedName name="BarTotal">GradientBar!$B$2</definedName>
+    <definedName name="MapBottomLeft">GradientMap!$B$4</definedName>
+    <definedName name="MapBottomRight">GradientMap!$B$5</definedName>
+    <definedName name="MapHeight">GradientMap!$B$7</definedName>
+    <definedName name="MapTopLeft">GradientMap!$B$2</definedName>
+    <definedName name="MapTopRight">GradientMap!$B$3</definedName>
+    <definedName name="MapVerticalStepL">GradientMap!$B$8</definedName>
+    <definedName name="MapVerticalStepR">GradientMap!$B$9</definedName>
+    <definedName name="MapWidth">GradientMap!$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Width</t>
   </si>
@@ -81,13 +85,17 @@
   <si>
     <t>BottomRight</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -138,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,6 +170,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -480,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58674667-26E3-48AC-A26A-6B2A59F0ECC9}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -569,11 +580,11 @@
         <v>1</v>
       </c>
       <c r="D2" s="6">
-        <f>TopLeft</f>
+        <f>MapTopLeft</f>
         <v>255</v>
       </c>
       <c r="E2" s="6">
-        <f>TopRight</f>
+        <f>MapTopRight</f>
         <v>160</v>
       </c>
       <c r="F2" s="6">
@@ -581,7 +592,7 @@
         <v>95</v>
       </c>
       <c r="G2" s="6">
-        <f>-F2/(Width-1)</f>
+        <f t="shared" ref="G2:G17" si="0">-F2/(MapWidth-1)</f>
         <v>-6.333333333333333</v>
       </c>
       <c r="H2" s="3">
@@ -596,59 +607,59 @@
         <v>248.66666666666666</v>
       </c>
       <c r="K2" s="7">
-        <f t="shared" ref="K2:X3" si="0">J2+$G2</f>
+        <f t="shared" ref="K2:X2" si="1">J2+$G2</f>
         <v>242.33333333333331</v>
       </c>
       <c r="L2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>235.99999999999997</v>
       </c>
       <c r="M2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>229.66666666666663</v>
       </c>
       <c r="N2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>223.33333333333329</v>
       </c>
       <c r="O2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>216.99999999999994</v>
       </c>
       <c r="P2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>210.6666666666666</v>
       </c>
       <c r="Q2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>204.33333333333326</v>
       </c>
       <c r="R2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>197.99999999999991</v>
       </c>
       <c r="S2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>191.66666666666657</v>
       </c>
       <c r="T2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>185.33333333333323</v>
       </c>
       <c r="U2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>178.99999999999989</v>
       </c>
       <c r="V2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>172.66666666666654</v>
       </c>
       <c r="W2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>166.3333333333332</v>
       </c>
       <c r="X2" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>159.99999999999986</v>
       </c>
       <c r="Y2" s="3">
@@ -666,86 +677,86 @@
         <v>2</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D17" si="1">D2-VerticalStepL</f>
+        <f t="shared" ref="D3:D17" si="2">D2-MapVerticalStepL</f>
         <v>239.33333333333334</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E17" si="2">E2-VerticalStepR</f>
+        <f t="shared" ref="E3:E17" si="3">E2-MapVerticalStepR</f>
         <v>152.66666666666666</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" ref="F3:F17" si="3">D3-E3</f>
+        <f t="shared" ref="F3:F17" si="4">D3-E3</f>
         <v>86.666666666666686</v>
       </c>
       <c r="G3" s="6">
-        <f>-F3/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-5.7777777777777795</v>
       </c>
       <c r="H3" s="3">
         <v>2</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3:I17" si="4">D3</f>
+        <f t="shared" ref="I3:I17" si="5">D3</f>
         <v>239.33333333333334</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:X3" si="5">I3+$G3</f>
+        <f t="shared" ref="J3:X3" si="6">I3+$G3</f>
         <v>233.55555555555557</v>
       </c>
       <c r="K3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>227.7777777777778</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>222.00000000000003</v>
       </c>
       <c r="M3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>216.22222222222226</v>
       </c>
       <c r="N3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>210.44444444444449</v>
       </c>
       <c r="O3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>204.66666666666671</v>
       </c>
       <c r="P3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>198.88888888888894</v>
       </c>
       <c r="Q3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>193.11111111111117</v>
       </c>
       <c r="R3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>187.3333333333334</v>
       </c>
       <c r="S3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>181.55555555555563</v>
       </c>
       <c r="T3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>175.77777777777786</v>
       </c>
       <c r="U3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>170.00000000000009</v>
       </c>
       <c r="V3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>164.22222222222231</v>
       </c>
       <c r="W3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>158.44444444444454</v>
       </c>
       <c r="X3" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>152.66666666666677</v>
       </c>
       <c r="Y3" s="3">
@@ -763,86 +774,86 @@
         <v>3</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>223.66666666666669</v>
       </c>
       <c r="E4" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145.33333333333331</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78.333333333333371</v>
       </c>
       <c r="G4" s="6">
-        <f>-F4/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-5.222222222222225</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>223.66666666666669</v>
       </c>
       <c r="J4" s="7">
-        <f t="shared" ref="J4:X4" si="6">I4+$G4</f>
+        <f t="shared" ref="J4:X4" si="7">I4+$G4</f>
         <v>218.44444444444446</v>
       </c>
       <c r="K4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>213.22222222222223</v>
       </c>
       <c r="L4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>208</v>
       </c>
       <c r="M4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>202.77777777777777</v>
       </c>
       <c r="N4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>197.55555555555554</v>
       </c>
       <c r="O4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>192.33333333333331</v>
       </c>
       <c r="P4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>187.11111111111109</v>
       </c>
       <c r="Q4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>181.88888888888886</v>
       </c>
       <c r="R4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>176.66666666666663</v>
       </c>
       <c r="S4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>171.4444444444444</v>
       </c>
       <c r="T4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>166.22222222222217</v>
       </c>
       <c r="U4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>160.99999999999994</v>
       </c>
       <c r="V4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>155.77777777777771</v>
       </c>
       <c r="W4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150.55555555555549</v>
       </c>
       <c r="X4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>145.33333333333326</v>
       </c>
       <c r="Y4" s="3">
@@ -860,86 +871,86 @@
         <v>4</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>208.00000000000003</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>137.99999999999997</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70.000000000000057</v>
       </c>
       <c r="G5" s="6">
-        <f>-F5/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-4.6666666666666705</v>
       </c>
       <c r="H5" s="3">
         <v>4</v>
       </c>
       <c r="I5" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>208.00000000000003</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" ref="J5:X5" si="7">I5+$G5</f>
+        <f t="shared" ref="J5:X5" si="8">I5+$G5</f>
         <v>203.33333333333337</v>
       </c>
       <c r="K5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>198.66666666666671</v>
       </c>
       <c r="L5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>194.00000000000006</v>
       </c>
       <c r="M5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>189.3333333333334</v>
       </c>
       <c r="N5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>184.66666666666674</v>
       </c>
       <c r="O5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>180.00000000000009</v>
       </c>
       <c r="P5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>175.33333333333343</v>
       </c>
       <c r="Q5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>170.66666666666677</v>
       </c>
       <c r="R5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>166.00000000000011</v>
       </c>
       <c r="S5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>161.33333333333346</v>
       </c>
       <c r="T5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>156.6666666666668</v>
       </c>
       <c r="U5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>152.00000000000014</v>
       </c>
       <c r="V5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>147.33333333333348</v>
       </c>
       <c r="W5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>142.66666666666683</v>
       </c>
       <c r="X5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>138.00000000000017</v>
       </c>
       <c r="Y5" s="3">
@@ -957,86 +968,86 @@
         <v>5</v>
       </c>
       <c r="D6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>192.33333333333337</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130.66666666666663</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61.666666666666742</v>
       </c>
       <c r="G6" s="6">
-        <f>-F6/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-4.111111111111116</v>
       </c>
       <c r="H6" s="3">
         <v>5</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>192.33333333333337</v>
       </c>
       <c r="J6" s="7">
-        <f t="shared" ref="J6:X6" si="8">I6+$G6</f>
+        <f t="shared" ref="J6:X6" si="9">I6+$G6</f>
         <v>188.22222222222226</v>
       </c>
       <c r="K6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>184.11111111111114</v>
       </c>
       <c r="L6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>180.00000000000003</v>
       </c>
       <c r="M6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>175.88888888888891</v>
       </c>
       <c r="N6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>171.7777777777778</v>
       </c>
       <c r="O6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>167.66666666666669</v>
       </c>
       <c r="P6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>163.55555555555557</v>
       </c>
       <c r="Q6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>159.44444444444446</v>
       </c>
       <c r="R6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>155.33333333333334</v>
       </c>
       <c r="S6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>151.22222222222223</v>
       </c>
       <c r="T6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>147.11111111111111</v>
       </c>
       <c r="U6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>143</v>
       </c>
       <c r="V6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>138.88888888888889</v>
       </c>
       <c r="W6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>134.77777777777777</v>
       </c>
       <c r="X6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>130.66666666666666</v>
       </c>
       <c r="Y6" s="3">
@@ -1054,86 +1065,86 @@
         <v>6</v>
       </c>
       <c r="D7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>176.66666666666671</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>123.3333333333333</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53.333333333333414</v>
       </c>
       <c r="G7" s="6">
-        <f>-F7/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-3.5555555555555611</v>
       </c>
       <c r="H7" s="3">
         <v>6</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>176.66666666666671</v>
       </c>
       <c r="J7" s="7">
-        <f t="shared" ref="J7:X7" si="9">I7+$G7</f>
+        <f t="shared" ref="J7:X7" si="10">I7+$G7</f>
         <v>173.11111111111114</v>
       </c>
       <c r="K7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>169.55555555555557</v>
       </c>
       <c r="L7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>166</v>
       </c>
       <c r="M7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>162.44444444444443</v>
       </c>
       <c r="N7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>158.88888888888886</v>
       </c>
       <c r="O7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>155.33333333333329</v>
       </c>
       <c r="P7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>151.77777777777771</v>
       </c>
       <c r="Q7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>148.22222222222214</v>
       </c>
       <c r="R7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>144.66666666666657</v>
       </c>
       <c r="S7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>141.111111111111</v>
       </c>
       <c r="T7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>137.55555555555543</v>
       </c>
       <c r="U7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>133.99999999999986</v>
       </c>
       <c r="V7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>130.44444444444429</v>
       </c>
       <c r="W7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>126.88888888888873</v>
       </c>
       <c r="X7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>123.33333333333317</v>
       </c>
       <c r="Y7" s="3">
@@ -1145,93 +1156,93 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <f>(TopLeft-BottomLeft)/(Height-1)</f>
+        <f>(MapTopLeft-MapBottomLeft)/(MapHeight-1)</f>
         <v>15.666666666666666</v>
       </c>
       <c r="C8" s="3">
         <v>7</v>
       </c>
       <c r="D8" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>161.00000000000006</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115.99999999999997</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45.000000000000085</v>
       </c>
       <c r="G8" s="6">
-        <f>-F8/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-3.0000000000000058</v>
       </c>
       <c r="H8" s="3">
         <v>7</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>161.00000000000006</v>
       </c>
       <c r="J8" s="7">
-        <f t="shared" ref="J8:X8" si="10">I8+$G8</f>
+        <f t="shared" ref="J8:X8" si="11">I8+$G8</f>
         <v>158.00000000000006</v>
       </c>
       <c r="K8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>155.00000000000006</v>
       </c>
       <c r="L8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>152.00000000000006</v>
       </c>
       <c r="M8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>149.00000000000006</v>
       </c>
       <c r="N8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>146.00000000000006</v>
       </c>
       <c r="O8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>143.00000000000006</v>
       </c>
       <c r="P8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>140.00000000000006</v>
       </c>
       <c r="Q8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>137.00000000000006</v>
       </c>
       <c r="R8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>134.00000000000006</v>
       </c>
       <c r="S8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>131.00000000000006</v>
       </c>
       <c r="T8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>128.00000000000006</v>
       </c>
       <c r="U8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>125.00000000000006</v>
       </c>
       <c r="V8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>122.00000000000006</v>
       </c>
       <c r="W8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>119.00000000000006</v>
       </c>
       <c r="X8" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>116.00000000000006</v>
       </c>
       <c r="Y8" s="3">
@@ -1243,93 +1254,93 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <f>(TopRight-BottomRight)/(Height - 1)</f>
+        <f>(MapTopRight-MapBottomRight)/(MapHeight - 1)</f>
         <v>7.333333333333333</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>145.3333333333334</v>
       </c>
       <c r="E9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108.66666666666664</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.666666666666757</v>
       </c>
       <c r="G9" s="6">
-        <f>-F9/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-2.4444444444444504</v>
       </c>
       <c r="H9" s="3">
         <v>8</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>145.3333333333334</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" ref="J9:X9" si="11">I9+$G9</f>
+        <f t="shared" ref="J9:X9" si="12">I9+$G9</f>
         <v>142.88888888888894</v>
       </c>
       <c r="K9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>140.44444444444449</v>
       </c>
       <c r="L9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>138.00000000000003</v>
       </c>
       <c r="M9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>135.55555555555557</v>
       </c>
       <c r="N9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>133.11111111111111</v>
       </c>
       <c r="O9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>130.66666666666666</v>
       </c>
       <c r="P9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>128.2222222222222</v>
       </c>
       <c r="Q9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>125.77777777777774</v>
       </c>
       <c r="R9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>123.33333333333329</v>
       </c>
       <c r="S9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>120.88888888888883</v>
       </c>
       <c r="T9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>118.44444444444437</v>
       </c>
       <c r="U9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>115.99999999999991</v>
       </c>
       <c r="V9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>113.55555555555546</v>
       </c>
       <c r="W9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>111.111111111111</v>
       </c>
       <c r="X9" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>108.66666666666654</v>
       </c>
       <c r="Y9" s="3">
@@ -1341,86 +1352,86 @@
         <v>9</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>129.66666666666674</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101.33333333333331</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28.333333333333428</v>
       </c>
       <c r="G10" s="6">
-        <f>-F10/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-1.8888888888888953</v>
       </c>
       <c r="H10" s="3">
         <v>9</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>129.66666666666674</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" ref="J10:X10" si="12">I10+$G10</f>
+        <f t="shared" ref="J10:X10" si="13">I10+$G10</f>
         <v>127.77777777777784</v>
       </c>
       <c r="K10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>125.88888888888894</v>
       </c>
       <c r="L10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>124.00000000000004</v>
       </c>
       <c r="M10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>122.11111111111114</v>
       </c>
       <c r="N10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>120.22222222222224</v>
       </c>
       <c r="O10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>118.33333333333334</v>
       </c>
       <c r="P10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>116.44444444444444</v>
       </c>
       <c r="Q10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>114.55555555555554</v>
       </c>
       <c r="R10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>112.66666666666664</v>
       </c>
       <c r="S10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>110.77777777777774</v>
       </c>
       <c r="T10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>108.88888888888884</v>
       </c>
       <c r="U10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>106.99999999999994</v>
       </c>
       <c r="V10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>105.11111111111104</v>
       </c>
       <c r="W10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>103.22222222222214</v>
       </c>
       <c r="X10" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>101.33333333333324</v>
       </c>
       <c r="Y10" s="3">
@@ -1432,86 +1443,86 @@
         <v>10</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>114.00000000000007</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93.999999999999986</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20.000000000000085</v>
       </c>
       <c r="G11" s="6">
-        <f>-F11/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-1.333333333333339</v>
       </c>
       <c r="H11" s="3">
         <v>10</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>114.00000000000007</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" ref="J11:X11" si="13">I11+$G11</f>
+        <f t="shared" ref="J11:X11" si="14">I11+$G11</f>
         <v>112.66666666666673</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>111.33333333333339</v>
       </c>
       <c r="L11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>110.00000000000004</v>
       </c>
       <c r="M11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>108.6666666666667</v>
       </c>
       <c r="N11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>107.33333333333336</v>
       </c>
       <c r="O11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>106.00000000000001</v>
       </c>
       <c r="P11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>104.66666666666667</v>
       </c>
       <c r="Q11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>103.33333333333333</v>
       </c>
       <c r="R11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>101.99999999999999</v>
       </c>
       <c r="S11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>100.66666666666664</v>
       </c>
       <c r="T11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>99.3333333333333</v>
       </c>
       <c r="U11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>97.999999999999957</v>
       </c>
       <c r="V11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>96.666666666666615</v>
       </c>
       <c r="W11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>95.333333333333272</v>
       </c>
       <c r="X11" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>93.999999999999929</v>
       </c>
       <c r="Y11" s="3">
@@ -1523,86 +1534,86 @@
         <v>11</v>
       </c>
       <c r="D12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>98.3333333333334</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86.666666666666657</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.666666666666742</v>
       </c>
       <c r="G12" s="6">
-        <f>-F12/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-0.77777777777778279</v>
       </c>
       <c r="H12" s="3">
         <v>11</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>98.3333333333334</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" ref="J12:X12" si="14">I12+$G12</f>
+        <f t="shared" ref="J12:X12" si="15">I12+$G12</f>
         <v>97.555555555555614</v>
       </c>
       <c r="K12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>96.777777777777828</v>
       </c>
       <c r="L12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>96.000000000000043</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>95.222222222222257</v>
       </c>
       <c r="N12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>94.444444444444471</v>
       </c>
       <c r="O12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>93.666666666666686</v>
       </c>
       <c r="P12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>92.8888888888889</v>
       </c>
       <c r="Q12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>92.111111111111114</v>
       </c>
       <c r="R12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>91.333333333333329</v>
       </c>
       <c r="S12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>90.555555555555543</v>
       </c>
       <c r="T12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>89.777777777777757</v>
       </c>
       <c r="U12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>88.999999999999972</v>
       </c>
       <c r="V12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>88.222222222222186</v>
       </c>
       <c r="W12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>87.4444444444444</v>
       </c>
       <c r="X12" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>86.666666666666615</v>
       </c>
       <c r="Y12" s="3">
@@ -1614,86 +1625,86 @@
         <v>12</v>
       </c>
       <c r="D13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82.666666666666728</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79.333333333333329</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.3333333333333997</v>
       </c>
       <c r="G13" s="6">
-        <f>-F13/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>-0.22222222222222665</v>
       </c>
       <c r="H13" s="3">
         <v>12</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82.666666666666728</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" ref="J13:X13" si="15">I13+$G13</f>
+        <f t="shared" ref="J13:X13" si="16">I13+$G13</f>
         <v>82.4444444444445</v>
       </c>
       <c r="K13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>82.222222222222271</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>82.000000000000043</v>
       </c>
       <c r="M13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>81.777777777777814</v>
       </c>
       <c r="N13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>81.555555555555586</v>
       </c>
       <c r="O13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>81.333333333333357</v>
       </c>
       <c r="P13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>81.111111111111128</v>
       </c>
       <c r="Q13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>80.8888888888889</v>
       </c>
       <c r="R13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>80.666666666666671</v>
       </c>
       <c r="S13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>80.444444444444443</v>
       </c>
       <c r="T13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>80.222222222222214</v>
       </c>
       <c r="U13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>79.999999999999986</v>
       </c>
       <c r="V13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>79.777777777777757</v>
       </c>
       <c r="W13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>79.555555555555529</v>
       </c>
       <c r="X13" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>79.3333333333333</v>
       </c>
       <c r="Y13" s="3">
@@ -1705,86 +1716,86 @@
         <v>13</v>
       </c>
       <c r="D14" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67.000000000000057</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.9999999999999432</v>
       </c>
       <c r="G14" s="6">
-        <f>-F14/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333332954</v>
       </c>
       <c r="H14" s="3">
         <v>13</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67.000000000000057</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" ref="J14:X14" si="16">I14+$G14</f>
+        <f t="shared" ref="J14:X14" si="17">I14+$G14</f>
         <v>67.333333333333385</v>
       </c>
       <c r="K14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>67.666666666666714</v>
       </c>
       <c r="L14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>68.000000000000043</v>
       </c>
       <c r="M14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>68.333333333333371</v>
       </c>
       <c r="N14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>68.6666666666667</v>
       </c>
       <c r="O14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>69.000000000000028</v>
       </c>
       <c r="P14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>69.333333333333357</v>
       </c>
       <c r="Q14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>69.666666666666686</v>
       </c>
       <c r="R14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.000000000000014</v>
       </c>
       <c r="S14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.333333333333343</v>
       </c>
       <c r="T14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.666666666666671</v>
       </c>
       <c r="U14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>71</v>
       </c>
       <c r="V14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>71.333333333333329</v>
       </c>
       <c r="W14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>71.666666666666657</v>
       </c>
       <c r="X14" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>71.999999999999986</v>
       </c>
       <c r="Y14" s="3">
@@ -1796,86 +1807,86 @@
         <v>14</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51.333333333333393</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64.666666666666671</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-13.333333333333279</v>
       </c>
       <c r="G15" s="6">
-        <f>-F15/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>0.88888888888888529</v>
       </c>
       <c r="H15" s="3">
         <v>14</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51.333333333333393</v>
       </c>
       <c r="J15" s="7">
-        <f t="shared" ref="J15:X15" si="17">I15+$G15</f>
+        <f t="shared" ref="J15:X15" si="18">I15+$G15</f>
         <v>52.222222222222278</v>
       </c>
       <c r="K15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>53.111111111111164</v>
       </c>
       <c r="L15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>54.00000000000005</v>
       </c>
       <c r="M15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>54.888888888888935</v>
       </c>
       <c r="N15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>55.777777777777821</v>
       </c>
       <c r="O15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>56.666666666666707</v>
       </c>
       <c r="P15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>57.555555555555593</v>
       </c>
       <c r="Q15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>58.444444444444478</v>
       </c>
       <c r="R15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>59.333333333333364</v>
       </c>
       <c r="S15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>60.22222222222225</v>
       </c>
       <c r="T15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>61.111111111111136</v>
       </c>
       <c r="U15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>62.000000000000021</v>
       </c>
       <c r="V15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>62.888888888888907</v>
       </c>
       <c r="W15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>63.777777777777793</v>
       </c>
       <c r="X15" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>64.666666666666671</v>
       </c>
       <c r="Y15" s="3">
@@ -1887,86 +1898,86 @@
         <v>15</v>
       </c>
       <c r="D16" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.666666666666728</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57.333333333333336</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-21.666666666666607</v>
       </c>
       <c r="G16" s="6">
-        <f>-F16/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>1.4444444444444404</v>
       </c>
       <c r="H16" s="3">
         <v>15</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35.666666666666728</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" ref="J16:X16" si="18">I16+$G16</f>
+        <f t="shared" ref="J16:X16" si="19">I16+$G16</f>
         <v>37.111111111111171</v>
       </c>
       <c r="K16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>38.555555555555614</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>40.000000000000057</v>
       </c>
       <c r="M16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>41.4444444444445</v>
       </c>
       <c r="N16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>42.888888888888943</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>44.333333333333385</v>
       </c>
       <c r="P16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>45.777777777777828</v>
       </c>
       <c r="Q16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>47.222222222222271</v>
       </c>
       <c r="R16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>48.666666666666714</v>
       </c>
       <c r="S16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>50.111111111111157</v>
       </c>
       <c r="T16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>51.5555555555556</v>
       </c>
       <c r="U16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>53.000000000000043</v>
       </c>
       <c r="V16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>54.444444444444485</v>
       </c>
       <c r="W16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>55.888888888888928</v>
       </c>
       <c r="X16" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>57.333333333333371</v>
       </c>
       <c r="Y16" s="3">
@@ -1978,86 +1989,86 @@
         <v>16</v>
       </c>
       <c r="D17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.000000000000064</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-29.999999999999936</v>
       </c>
       <c r="G17" s="6">
-        <f>-F17/(Width-1)</f>
+        <f t="shared" si="0"/>
         <v>1.9999999999999958</v>
       </c>
       <c r="H17" s="3">
         <v>16</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.000000000000064</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" ref="J17:X17" si="19">I17+$G17</f>
+        <f t="shared" ref="J17:X17" si="20">I17+$G17</f>
         <v>22.00000000000006</v>
       </c>
       <c r="K17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>24.000000000000057</v>
       </c>
       <c r="L17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>26.000000000000053</v>
       </c>
       <c r="M17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>28.00000000000005</v>
       </c>
       <c r="N17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30.000000000000046</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>32.000000000000043</v>
       </c>
       <c r="P17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>34.000000000000036</v>
       </c>
       <c r="Q17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>36.000000000000028</v>
       </c>
       <c r="R17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>38.000000000000021</v>
       </c>
       <c r="S17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>40.000000000000014</v>
       </c>
       <c r="T17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>42.000000000000007</v>
       </c>
       <c r="U17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>44</v>
       </c>
       <c r="V17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>45.999999999999993</v>
       </c>
       <c r="W17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>47.999999999999986</v>
       </c>
       <c r="X17" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>49.999999999999979</v>
       </c>
       <c r="Y17" s="3">
@@ -2115,6 +2126,417 @@
         <v>16</v>
       </c>
       <c r="Y18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C95354-AFC5-4BDD-8CDC-A4CA5B3B0235}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="4" style="1" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="1"/>
+    <col min="8" max="10" width="4" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3">
+        <v>1</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8">
+        <f>256*6</f>
+        <v>1536</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <f>MapTopLeft</f>
+        <v>255</v>
+      </c>
+      <c r="E2" s="6">
+        <f>MapTopRight</f>
+        <v>160</v>
+      </c>
+      <c r="F2" s="6">
+        <f>D2-E2</f>
+        <v>95</v>
+      </c>
+      <c r="G2" s="6">
+        <f t="shared" ref="G2:G12" si="0">-F2/(MapWidth-1)</f>
+        <v>-6.333333333333333</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <f>D2</f>
+        <v>255</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D12" si="1">D2-MapVerticalStepL</f>
+        <v>239.33333333333334</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E12" si="2">E2-MapVerticalStepR</f>
+        <v>152.66666666666666</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F12" si="3">D3-E3</f>
+        <v>86.666666666666686</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" si="0"/>
+        <v>-5.7777777777777795</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I12" si="4">D3</f>
+        <v>239.33333333333334</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <f>BarHeight/BarTotal</f>
+        <v>1.953125E-2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="e">
+        <f>#REF!-MapVerticalStepL</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E4" s="6" t="e">
+        <f>#REF!-MapVerticalStepR</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F4" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G4" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H4" s="3">
+        <v>7</v>
+      </c>
+      <c r="I4" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J4" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="e">
+        <f>#REF!-MapVerticalStepL</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E5" s="6" t="e">
+        <f>#REF!-MapVerticalStepR</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F5" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G5" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H5" s="3">
+        <v>9</v>
+      </c>
+      <c r="I5" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E6" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="F6" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G6" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
+      <c r="I6" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J6" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="F7" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G7" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H7" s="3">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J7" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E8" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="F8" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G8" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H8" s="3">
+        <v>12</v>
+      </c>
+      <c r="I8" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J8" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E9" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="F9" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G9" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H9" s="3">
+        <v>13</v>
+      </c>
+      <c r="I9" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E10" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="F10" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G10" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H10" s="3">
+        <v>14</v>
+      </c>
+      <c r="I10" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J10" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="F11" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G11" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H11" s="3">
+        <v>15</v>
+      </c>
+      <c r="I11" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J11" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E12" s="6" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="F12" s="6" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G12" s="6" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H12" s="3">
+        <v>16</v>
+      </c>
+      <c r="I12" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J12" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>